<commit_message>
more bots config; web parser tunnel
</commit_message>
<xml_diff>
--- a/_bots/gorkathebot/gorkathebot.xlsx
+++ b/_bots/gorkathebot/gorkathebot.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="89">
   <si>
     <t xml:space="preserve">BOTBASIC</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">VERSION</t>
   </si>
   <si>
-    <t xml:space="preserve">0.1.3</t>
+    <t xml:space="preserve">0.1.4</t>
   </si>
   <si>
     <t xml:space="preserve">gorkathebot</t>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t xml:space="preserve">A person called {username} is a fool if reading this line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prank2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I get more of your time that you of mine</t>
   </si>
   <si>
     <t xml:space="preserve">silly1</t>
@@ -265,7 +271,7 @@
     <t xml:space="preserve">prank</t>
   </si>
   <si>
-    <t xml:space="preserve">SET tryToLaugh prank1</t>
+    <t xml:space="preserve">SET tryToLaugh prank2</t>
   </si>
   <si>
     <t xml:space="preserve">RETURN</t>
@@ -515,14 +521,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ82"/>
+  <dimension ref="A1:AMJ83"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23819,6 +23825,12 @@
       <c r="ALP25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="D26" s="0"/>
       <c r="E26" s="0"/>
       <c r="F26" s="0"/>
@@ -26828,24 +26840,19 @@
       <c r="ALP28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="9"/>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
+      <c r="G29" s="0"/>
+      <c r="H29" s="0"/>
+      <c r="I29" s="0"/>
+      <c r="J29" s="0"/>
+      <c r="K29" s="0"/>
+      <c r="L29" s="0"/>
+      <c r="M29" s="0"/>
+      <c r="N29" s="0"/>
+      <c r="O29" s="0"/>
+      <c r="P29" s="0"/>
       <c r="Q29" s="0"/>
       <c r="R29" s="0"/>
       <c r="S29" s="0"/>
@@ -27836,32 +27843,24 @@
       <c r="ALP29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="0"/>
-      <c r="C30" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="0"/>
-      <c r="E30" s="1" t="s">
+      <c r="A30" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H30" s="0"/>
-      <c r="I30" s="0"/>
-      <c r="J30" s="0"/>
-      <c r="K30" s="0"/>
-      <c r="L30" s="0"/>
-      <c r="M30" s="0"/>
-      <c r="N30" s="0"/>
-      <c r="O30" s="0"/>
-      <c r="P30" s="0"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="9"/>
       <c r="Q30" s="0"/>
       <c r="R30" s="0"/>
       <c r="S30" s="0"/>
@@ -28851,14 +28850,24 @@
       <c r="ALO30" s="0"/>
       <c r="ALP30" s="0"/>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0"/>
+    <row r="31" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B31" s="0"/>
-      <c r="C31" s="0"/>
+      <c r="C31" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D31" s="0"/>
-      <c r="E31" s="0"/>
-      <c r="F31" s="0"/>
-      <c r="G31" s="0"/>
+      <c r="E31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H31" s="0"/>
       <c r="I31" s="0"/>
       <c r="J31" s="0"/>
@@ -31869,25 +31878,23 @@
       <c r="ALO33" s="0"/>
       <c r="ALP33" s="0"/>
     </row>
-    <row r="34" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="9"/>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0"/>
+      <c r="B34" s="0"/>
+      <c r="C34" s="0"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
+      <c r="F34" s="0"/>
+      <c r="G34" s="0"/>
+      <c r="H34" s="0"/>
+      <c r="I34" s="0"/>
+      <c r="J34" s="0"/>
+      <c r="K34" s="0"/>
+      <c r="L34" s="0"/>
+      <c r="M34" s="0"/>
+      <c r="N34" s="0"/>
+      <c r="O34" s="0"/>
+      <c r="P34" s="0"/>
       <c r="Q34" s="0"/>
       <c r="R34" s="0"/>
       <c r="S34" s="0"/>
@@ -32878,26 +32885,24 @@
       <c r="ALP34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>9</v>
+      <c r="A35" s="7" t="s">
+        <v>47</v>
       </c>
-      <c r="B35" s="0"/>
-      <c r="C35" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="0"/>
-      <c r="E35" s="0"/>
-      <c r="F35" s="0"/>
-      <c r="G35" s="0"/>
-      <c r="H35" s="0"/>
-      <c r="I35" s="0"/>
-      <c r="J35" s="0"/>
-      <c r="K35" s="0"/>
-      <c r="L35" s="0"/>
-      <c r="M35" s="0"/>
-      <c r="N35" s="0"/>
-      <c r="O35" s="0"/>
-      <c r="P35" s="0"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="9"/>
       <c r="Q35" s="0"/>
       <c r="R35" s="0"/>
       <c r="S35" s="0"/>
@@ -33887,10 +33892,14 @@
       <c r="ALO35" s="0"/>
       <c r="ALP35" s="0"/>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0"/>
+    <row r="36" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B36" s="0"/>
-      <c r="C36" s="0"/>
+      <c r="C36" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D36" s="0"/>
       <c r="E36" s="0"/>
       <c r="F36" s="0"/>
@@ -36905,25 +36914,23 @@
       <c r="ALO38" s="0"/>
       <c r="ALP38" s="0"/>
     </row>
-    <row r="39" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="9"/>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0"/>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
+      <c r="F39" s="0"/>
+      <c r="G39" s="0"/>
+      <c r="H39" s="0"/>
+      <c r="I39" s="0"/>
+      <c r="J39" s="0"/>
+      <c r="K39" s="0"/>
+      <c r="L39" s="0"/>
+      <c r="M39" s="0"/>
+      <c r="N39" s="0"/>
+      <c r="O39" s="0"/>
+      <c r="P39" s="0"/>
       <c r="Q39" s="0"/>
       <c r="R39" s="0"/>
       <c r="S39" s="0"/>
@@ -37914,32 +37921,24 @@
       <c r="ALP39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>9</v>
+      <c r="A40" s="7" t="s">
+        <v>48</v>
       </c>
-      <c r="B40" s="0"/>
-      <c r="C40" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D40" s="0"/>
-      <c r="E40" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H40" s="0"/>
-      <c r="I40" s="0"/>
-      <c r="J40" s="0"/>
-      <c r="K40" s="0"/>
-      <c r="L40" s="0"/>
-      <c r="M40" s="0"/>
-      <c r="N40" s="0"/>
-      <c r="O40" s="0"/>
-      <c r="P40" s="0"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="9"/>
       <c r="Q40" s="0"/>
       <c r="R40" s="0"/>
       <c r="S40" s="0"/>
@@ -38929,14 +38928,24 @@
       <c r="ALO40" s="0"/>
       <c r="ALP40" s="0"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0"/>
+    <row r="41" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B41" s="0"/>
-      <c r="C41" s="0"/>
+      <c r="C41" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D41" s="0"/>
-      <c r="E41" s="0"/>
-      <c r="F41" s="0"/>
-      <c r="G41" s="0"/>
+      <c r="E41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H41" s="0"/>
       <c r="I41" s="0"/>
       <c r="J41" s="0"/>
@@ -39935,19 +39944,13 @@
       <c r="ALO41" s="0"/>
       <c r="ALP41" s="0"/>
     </row>
-    <row r="42" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>47</v>
-      </c>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0"/>
       <c r="B42" s="0"/>
       <c r="C42" s="0"/>
       <c r="D42" s="0"/>
-      <c r="E42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="E42" s="0"/>
+      <c r="F42" s="0"/>
       <c r="G42" s="0"/>
       <c r="H42" s="0"/>
       <c r="I42" s="0"/>
@@ -40949,16 +40952,16 @@
     </row>
     <row r="43" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B43" s="0"/>
       <c r="C43" s="0"/>
       <c r="D43" s="0"/>
       <c r="E43" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G43" s="0"/>
       <c r="H43" s="0"/>
@@ -41961,16 +41964,16 @@
     </row>
     <row r="44" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44" s="0"/>
       <c r="C44" s="0"/>
       <c r="D44" s="0"/>
       <c r="E44" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G44" s="0"/>
       <c r="H44" s="0"/>
@@ -42971,13 +42974,19 @@
       <c r="ALO44" s="0"/>
       <c r="ALP44" s="0"/>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0"/>
+    <row r="45" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="B45" s="0"/>
       <c r="C45" s="0"/>
       <c r="D45" s="0"/>
-      <c r="E45" s="0"/>
-      <c r="F45" s="0"/>
+      <c r="E45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="G45" s="0"/>
       <c r="H45" s="0"/>
       <c r="I45" s="0"/>
@@ -45989,25 +45998,23 @@
       <c r="ALO47" s="0"/>
       <c r="ALP47" s="0"/>
     </row>
-    <row r="48" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="9"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="9"/>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0"/>
+      <c r="B48" s="0"/>
+      <c r="C48" s="0"/>
+      <c r="D48" s="0"/>
+      <c r="E48" s="0"/>
+      <c r="F48" s="0"/>
+      <c r="G48" s="0"/>
+      <c r="H48" s="0"/>
+      <c r="I48" s="0"/>
+      <c r="J48" s="0"/>
+      <c r="K48" s="0"/>
+      <c r="L48" s="0"/>
+      <c r="M48" s="0"/>
+      <c r="N48" s="0"/>
+      <c r="O48" s="0"/>
+      <c r="P48" s="0"/>
       <c r="Q48" s="0"/>
       <c r="R48" s="0"/>
       <c r="S48" s="0"/>
@@ -46998,28 +47005,24 @@
       <c r="ALP48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
-        <v>7</v>
+      <c r="A49" s="7" t="s">
+        <v>58</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" s="0"/>
-      <c r="E49" s="0"/>
-      <c r="F49" s="0"/>
-      <c r="G49" s="0"/>
-      <c r="H49" s="0"/>
-      <c r="I49" s="0"/>
-      <c r="J49" s="0"/>
-      <c r="K49" s="0"/>
-      <c r="L49" s="0"/>
-      <c r="M49" s="0"/>
-      <c r="N49" s="0"/>
-      <c r="O49" s="0"/>
-      <c r="P49" s="0"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="9"/>
       <c r="Q49" s="0"/>
       <c r="R49" s="0"/>
       <c r="S49" s="0"/>
@@ -48009,10 +48012,16 @@
       <c r="ALO49" s="0"/>
       <c r="ALP49" s="0"/>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0"/>
-      <c r="B50" s="0"/>
-      <c r="C50" s="0"/>
+    <row r="50" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="D50" s="0"/>
       <c r="E50" s="0"/>
       <c r="F50" s="0"/>
@@ -51027,25 +51036,22 @@
       <c r="ALO52" s="0"/>
       <c r="ALP52" s="0"/>
     </row>
-    <row r="53" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>59</v>
-      </c>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0"/>
+      <c r="B53" s="0"/>
+      <c r="C53" s="0"/>
       <c r="D53" s="0"/>
       <c r="E53" s="0"/>
       <c r="F53" s="0"/>
+      <c r="G53" s="0"/>
       <c r="H53" s="0"/>
       <c r="I53" s="0"/>
       <c r="J53" s="0"/>
+      <c r="K53" s="0"/>
       <c r="L53" s="0"/>
       <c r="M53" s="0"/>
       <c r="N53" s="0"/>
+      <c r="O53" s="0"/>
       <c r="P53" s="0"/>
       <c r="Q53" s="0"/>
       <c r="R53" s="0"/>
@@ -52037,8 +52043,14 @@
       <c r="ALP53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="C54" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D54" s="0"/>
       <c r="E54" s="0"/>
@@ -53040,6 +53052,9 @@
       <c r="ALP54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="D55" s="0"/>
       <c r="E55" s="0"/>
       <c r="F55" s="0"/>
@@ -54040,15 +54055,6 @@
       <c r="ALP55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="D56" s="0"/>
       <c r="E56" s="0"/>
       <c r="F56" s="0"/>
@@ -55048,125 +55054,1134 @@
       <c r="ALO56" s="0"/>
       <c r="ALP56" s="0"/>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="1" t="s">
+    <row r="57" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C57" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" s="0"/>
+      <c r="E57" s="0"/>
+      <c r="F57" s="0"/>
+      <c r="H57" s="0"/>
+      <c r="I57" s="0"/>
+      <c r="J57" s="0"/>
+      <c r="L57" s="0"/>
+      <c r="M57" s="0"/>
+      <c r="N57" s="0"/>
+      <c r="P57" s="0"/>
+      <c r="Q57" s="0"/>
+      <c r="R57" s="0"/>
+      <c r="S57" s="0"/>
+      <c r="T57" s="0"/>
+      <c r="U57" s="0"/>
+      <c r="V57" s="0"/>
+      <c r="W57" s="0"/>
+      <c r="X57" s="0"/>
+      <c r="Y57" s="0"/>
+      <c r="Z57" s="0"/>
+      <c r="AA57" s="0"/>
+      <c r="AB57" s="0"/>
+      <c r="AC57" s="0"/>
+      <c r="AD57" s="0"/>
+      <c r="AE57" s="0"/>
+      <c r="AF57" s="0"/>
+      <c r="AG57" s="0"/>
+      <c r="AH57" s="0"/>
+      <c r="AI57" s="0"/>
+      <c r="AJ57" s="0"/>
+      <c r="AK57" s="0"/>
+      <c r="AL57" s="0"/>
+      <c r="AM57" s="0"/>
+      <c r="AN57" s="0"/>
+      <c r="AO57" s="0"/>
+      <c r="AP57" s="0"/>
+      <c r="AQ57" s="0"/>
+      <c r="AR57" s="0"/>
+      <c r="AS57" s="0"/>
+      <c r="AT57" s="0"/>
+      <c r="AU57" s="0"/>
+      <c r="AV57" s="0"/>
+      <c r="AW57" s="0"/>
+      <c r="AX57" s="0"/>
+      <c r="AY57" s="0"/>
+      <c r="AZ57" s="0"/>
+      <c r="BA57" s="0"/>
+      <c r="BB57" s="0"/>
+      <c r="BC57" s="0"/>
+      <c r="BD57" s="0"/>
+      <c r="BE57" s="0"/>
+      <c r="BF57" s="0"/>
+      <c r="BG57" s="0"/>
+      <c r="BH57" s="0"/>
+      <c r="BI57" s="0"/>
+      <c r="BJ57" s="0"/>
+      <c r="BK57" s="0"/>
+      <c r="BL57" s="0"/>
+      <c r="BM57" s="0"/>
+      <c r="BN57" s="0"/>
+      <c r="BO57" s="0"/>
+      <c r="BP57" s="0"/>
+      <c r="BQ57" s="0"/>
+      <c r="BR57" s="0"/>
+      <c r="BS57" s="0"/>
+      <c r="BT57" s="0"/>
+      <c r="BU57" s="0"/>
+      <c r="BV57" s="0"/>
+      <c r="BW57" s="0"/>
+      <c r="BX57" s="0"/>
+      <c r="BY57" s="0"/>
+      <c r="BZ57" s="0"/>
+      <c r="CA57" s="0"/>
+      <c r="CB57" s="0"/>
+      <c r="CC57" s="0"/>
+      <c r="CD57" s="0"/>
+      <c r="CE57" s="0"/>
+      <c r="CF57" s="0"/>
+      <c r="CG57" s="0"/>
+      <c r="CH57" s="0"/>
+      <c r="CI57" s="0"/>
+      <c r="CJ57" s="0"/>
+      <c r="CK57" s="0"/>
+      <c r="CL57" s="0"/>
+      <c r="CM57" s="0"/>
+      <c r="CN57" s="0"/>
+      <c r="CO57" s="0"/>
+      <c r="CP57" s="0"/>
+      <c r="CQ57" s="0"/>
+      <c r="CR57" s="0"/>
+      <c r="CS57" s="0"/>
+      <c r="CT57" s="0"/>
+      <c r="CU57" s="0"/>
+      <c r="CV57" s="0"/>
+      <c r="CW57" s="0"/>
+      <c r="CX57" s="0"/>
+      <c r="CY57" s="0"/>
+      <c r="CZ57" s="0"/>
+      <c r="DA57" s="0"/>
+      <c r="DB57" s="0"/>
+      <c r="DC57" s="0"/>
+      <c r="DD57" s="0"/>
+      <c r="DE57" s="0"/>
+      <c r="DF57" s="0"/>
+      <c r="DG57" s="0"/>
+      <c r="DH57" s="0"/>
+      <c r="DI57" s="0"/>
+      <c r="DJ57" s="0"/>
+      <c r="DK57" s="0"/>
+      <c r="DL57" s="0"/>
+      <c r="DM57" s="0"/>
+      <c r="DN57" s="0"/>
+      <c r="DO57" s="0"/>
+      <c r="DP57" s="0"/>
+      <c r="DQ57" s="0"/>
+      <c r="DR57" s="0"/>
+      <c r="DS57" s="0"/>
+      <c r="DT57" s="0"/>
+      <c r="DU57" s="0"/>
+      <c r="DV57" s="0"/>
+      <c r="DW57" s="0"/>
+      <c r="DX57" s="0"/>
+      <c r="DY57" s="0"/>
+      <c r="DZ57" s="0"/>
+      <c r="EA57" s="0"/>
+      <c r="EB57" s="0"/>
+      <c r="EC57" s="0"/>
+      <c r="ED57" s="0"/>
+      <c r="EE57" s="0"/>
+      <c r="EF57" s="0"/>
+      <c r="EG57" s="0"/>
+      <c r="EH57" s="0"/>
+      <c r="EI57" s="0"/>
+      <c r="EJ57" s="0"/>
+      <c r="EK57" s="0"/>
+      <c r="EL57" s="0"/>
+      <c r="EM57" s="0"/>
+      <c r="EN57" s="0"/>
+      <c r="EO57" s="0"/>
+      <c r="EP57" s="0"/>
+      <c r="EQ57" s="0"/>
+      <c r="ER57" s="0"/>
+      <c r="ES57" s="0"/>
+      <c r="ET57" s="0"/>
+      <c r="EU57" s="0"/>
+      <c r="EV57" s="0"/>
+      <c r="EW57" s="0"/>
+      <c r="EX57" s="0"/>
+      <c r="EY57" s="0"/>
+      <c r="EZ57" s="0"/>
+      <c r="FA57" s="0"/>
+      <c r="FB57" s="0"/>
+      <c r="FC57" s="0"/>
+      <c r="FD57" s="0"/>
+      <c r="FE57" s="0"/>
+      <c r="FF57" s="0"/>
+      <c r="FG57" s="0"/>
+      <c r="FH57" s="0"/>
+      <c r="FI57" s="0"/>
+      <c r="FJ57" s="0"/>
+      <c r="FK57" s="0"/>
+      <c r="FL57" s="0"/>
+      <c r="FM57" s="0"/>
+      <c r="FN57" s="0"/>
+      <c r="FO57" s="0"/>
+      <c r="FP57" s="0"/>
+      <c r="FQ57" s="0"/>
+      <c r="FR57" s="0"/>
+      <c r="FS57" s="0"/>
+      <c r="FT57" s="0"/>
+      <c r="FU57" s="0"/>
+      <c r="FV57" s="0"/>
+      <c r="FW57" s="0"/>
+      <c r="FX57" s="0"/>
+      <c r="FY57" s="0"/>
+      <c r="FZ57" s="0"/>
+      <c r="GA57" s="0"/>
+      <c r="GB57" s="0"/>
+      <c r="GC57" s="0"/>
+      <c r="GD57" s="0"/>
+      <c r="GE57" s="0"/>
+      <c r="GF57" s="0"/>
+      <c r="GG57" s="0"/>
+      <c r="GH57" s="0"/>
+      <c r="GI57" s="0"/>
+      <c r="GJ57" s="0"/>
+      <c r="GK57" s="0"/>
+      <c r="GL57" s="0"/>
+      <c r="GM57" s="0"/>
+      <c r="GN57" s="0"/>
+      <c r="GO57" s="0"/>
+      <c r="GP57" s="0"/>
+      <c r="GQ57" s="0"/>
+      <c r="GR57" s="0"/>
+      <c r="GS57" s="0"/>
+      <c r="GT57" s="0"/>
+      <c r="GU57" s="0"/>
+      <c r="GV57" s="0"/>
+      <c r="GW57" s="0"/>
+      <c r="GX57" s="0"/>
+      <c r="GY57" s="0"/>
+      <c r="GZ57" s="0"/>
+      <c r="HA57" s="0"/>
+      <c r="HB57" s="0"/>
+      <c r="HC57" s="0"/>
+      <c r="HD57" s="0"/>
+      <c r="HE57" s="0"/>
+      <c r="HF57" s="0"/>
+      <c r="HG57" s="0"/>
+      <c r="HH57" s="0"/>
+      <c r="HI57" s="0"/>
+      <c r="HJ57" s="0"/>
+      <c r="HK57" s="0"/>
+      <c r="HL57" s="0"/>
+      <c r="HM57" s="0"/>
+      <c r="HN57" s="0"/>
+      <c r="HO57" s="0"/>
+      <c r="HP57" s="0"/>
+      <c r="HQ57" s="0"/>
+      <c r="HR57" s="0"/>
+      <c r="HS57" s="0"/>
+      <c r="HT57" s="0"/>
+      <c r="HU57" s="0"/>
+      <c r="HV57" s="0"/>
+      <c r="HW57" s="0"/>
+      <c r="HX57" s="0"/>
+      <c r="HY57" s="0"/>
+      <c r="HZ57" s="0"/>
+      <c r="IA57" s="0"/>
+      <c r="IB57" s="0"/>
+      <c r="IC57" s="0"/>
+      <c r="ID57" s="0"/>
+      <c r="IE57" s="0"/>
+      <c r="IF57" s="0"/>
+      <c r="IG57" s="0"/>
+      <c r="IH57" s="0"/>
+      <c r="II57" s="0"/>
+      <c r="IJ57" s="0"/>
+      <c r="IK57" s="0"/>
+      <c r="IL57" s="0"/>
+      <c r="IM57" s="0"/>
+      <c r="IN57" s="0"/>
+      <c r="IO57" s="0"/>
+      <c r="IP57" s="0"/>
+      <c r="IQ57" s="0"/>
+      <c r="IR57" s="0"/>
+      <c r="IS57" s="0"/>
+      <c r="IT57" s="0"/>
+      <c r="IU57" s="0"/>
+      <c r="IV57" s="0"/>
+      <c r="IW57" s="0"/>
+      <c r="IX57" s="0"/>
+      <c r="IY57" s="0"/>
+      <c r="IZ57" s="0"/>
+      <c r="JA57" s="0"/>
+      <c r="JB57" s="0"/>
+      <c r="JC57" s="0"/>
+      <c r="JD57" s="0"/>
+      <c r="JE57" s="0"/>
+      <c r="JF57" s="0"/>
+      <c r="JG57" s="0"/>
+      <c r="JH57" s="0"/>
+      <c r="JI57" s="0"/>
+      <c r="JJ57" s="0"/>
+      <c r="JK57" s="0"/>
+      <c r="JL57" s="0"/>
+      <c r="JM57" s="0"/>
+      <c r="JN57" s="0"/>
+      <c r="JO57" s="0"/>
+      <c r="JP57" s="0"/>
+      <c r="JQ57" s="0"/>
+      <c r="JR57" s="0"/>
+      <c r="JS57" s="0"/>
+      <c r="JT57" s="0"/>
+      <c r="JU57" s="0"/>
+      <c r="JV57" s="0"/>
+      <c r="JW57" s="0"/>
+      <c r="JX57" s="0"/>
+      <c r="JY57" s="0"/>
+      <c r="JZ57" s="0"/>
+      <c r="KA57" s="0"/>
+      <c r="KB57" s="0"/>
+      <c r="KC57" s="0"/>
+      <c r="KD57" s="0"/>
+      <c r="KE57" s="0"/>
+      <c r="KF57" s="0"/>
+      <c r="KG57" s="0"/>
+      <c r="KH57" s="0"/>
+      <c r="KI57" s="0"/>
+      <c r="KJ57" s="0"/>
+      <c r="KK57" s="0"/>
+      <c r="KL57" s="0"/>
+      <c r="KM57" s="0"/>
+      <c r="KN57" s="0"/>
+      <c r="KO57" s="0"/>
+      <c r="KP57" s="0"/>
+      <c r="KQ57" s="0"/>
+      <c r="KR57" s="0"/>
+      <c r="KS57" s="0"/>
+      <c r="KT57" s="0"/>
+      <c r="KU57" s="0"/>
+      <c r="KV57" s="0"/>
+      <c r="KW57" s="0"/>
+      <c r="KX57" s="0"/>
+      <c r="KY57" s="0"/>
+      <c r="KZ57" s="0"/>
+      <c r="LA57" s="0"/>
+      <c r="LB57" s="0"/>
+      <c r="LC57" s="0"/>
+      <c r="LD57" s="0"/>
+      <c r="LE57" s="0"/>
+      <c r="LF57" s="0"/>
+      <c r="LG57" s="0"/>
+      <c r="LH57" s="0"/>
+      <c r="LI57" s="0"/>
+      <c r="LJ57" s="0"/>
+      <c r="LK57" s="0"/>
+      <c r="LL57" s="0"/>
+      <c r="LM57" s="0"/>
+      <c r="LN57" s="0"/>
+      <c r="LO57" s="0"/>
+      <c r="LP57" s="0"/>
+      <c r="LQ57" s="0"/>
+      <c r="LR57" s="0"/>
+      <c r="LS57" s="0"/>
+      <c r="LT57" s="0"/>
+      <c r="LU57" s="0"/>
+      <c r="LV57" s="0"/>
+      <c r="LW57" s="0"/>
+      <c r="LX57" s="0"/>
+      <c r="LY57" s="0"/>
+      <c r="LZ57" s="0"/>
+      <c r="MA57" s="0"/>
+      <c r="MB57" s="0"/>
+      <c r="MC57" s="0"/>
+      <c r="MD57" s="0"/>
+      <c r="ME57" s="0"/>
+      <c r="MF57" s="0"/>
+      <c r="MG57" s="0"/>
+      <c r="MH57" s="0"/>
+      <c r="MI57" s="0"/>
+      <c r="MJ57" s="0"/>
+      <c r="MK57" s="0"/>
+      <c r="ML57" s="0"/>
+      <c r="MM57" s="0"/>
+      <c r="MN57" s="0"/>
+      <c r="MO57" s="0"/>
+      <c r="MP57" s="0"/>
+      <c r="MQ57" s="0"/>
+      <c r="MR57" s="0"/>
+      <c r="MS57" s="0"/>
+      <c r="MT57" s="0"/>
+      <c r="MU57" s="0"/>
+      <c r="MV57" s="0"/>
+      <c r="MW57" s="0"/>
+      <c r="MX57" s="0"/>
+      <c r="MY57" s="0"/>
+      <c r="MZ57" s="0"/>
+      <c r="NA57" s="0"/>
+      <c r="NB57" s="0"/>
+      <c r="NC57" s="0"/>
+      <c r="ND57" s="0"/>
+      <c r="NE57" s="0"/>
+      <c r="NF57" s="0"/>
+      <c r="NG57" s="0"/>
+      <c r="NH57" s="0"/>
+      <c r="NI57" s="0"/>
+      <c r="NJ57" s="0"/>
+      <c r="NK57" s="0"/>
+      <c r="NL57" s="0"/>
+      <c r="NM57" s="0"/>
+      <c r="NN57" s="0"/>
+      <c r="NO57" s="0"/>
+      <c r="NP57" s="0"/>
+      <c r="NQ57" s="0"/>
+      <c r="NR57" s="0"/>
+      <c r="NS57" s="0"/>
+      <c r="NT57" s="0"/>
+      <c r="NU57" s="0"/>
+      <c r="NV57" s="0"/>
+      <c r="NW57" s="0"/>
+      <c r="NX57" s="0"/>
+      <c r="NY57" s="0"/>
+      <c r="NZ57" s="0"/>
+      <c r="OA57" s="0"/>
+      <c r="OB57" s="0"/>
+      <c r="OC57" s="0"/>
+      <c r="OD57" s="0"/>
+      <c r="OE57" s="0"/>
+      <c r="OF57" s="0"/>
+      <c r="OG57" s="0"/>
+      <c r="OH57" s="0"/>
+      <c r="OI57" s="0"/>
+      <c r="OJ57" s="0"/>
+      <c r="OK57" s="0"/>
+      <c r="OL57" s="0"/>
+      <c r="OM57" s="0"/>
+      <c r="ON57" s="0"/>
+      <c r="OO57" s="0"/>
+      <c r="OP57" s="0"/>
+      <c r="OQ57" s="0"/>
+      <c r="OR57" s="0"/>
+      <c r="OS57" s="0"/>
+      <c r="OT57" s="0"/>
+      <c r="OU57" s="0"/>
+      <c r="OV57" s="0"/>
+      <c r="OW57" s="0"/>
+      <c r="OX57" s="0"/>
+      <c r="OY57" s="0"/>
+      <c r="OZ57" s="0"/>
+      <c r="PA57" s="0"/>
+      <c r="PB57" s="0"/>
+      <c r="PC57" s="0"/>
+      <c r="PD57" s="0"/>
+      <c r="PE57" s="0"/>
+      <c r="PF57" s="0"/>
+      <c r="PG57" s="0"/>
+      <c r="PH57" s="0"/>
+      <c r="PI57" s="0"/>
+      <c r="PJ57" s="0"/>
+      <c r="PK57" s="0"/>
+      <c r="PL57" s="0"/>
+      <c r="PM57" s="0"/>
+      <c r="PN57" s="0"/>
+      <c r="PO57" s="0"/>
+      <c r="PP57" s="0"/>
+      <c r="PQ57" s="0"/>
+      <c r="PR57" s="0"/>
+      <c r="PS57" s="0"/>
+      <c r="PT57" s="0"/>
+      <c r="PU57" s="0"/>
+      <c r="PV57" s="0"/>
+      <c r="PW57" s="0"/>
+      <c r="PX57" s="0"/>
+      <c r="PY57" s="0"/>
+      <c r="PZ57" s="0"/>
+      <c r="QA57" s="0"/>
+      <c r="QB57" s="0"/>
+      <c r="QC57" s="0"/>
+      <c r="QD57" s="0"/>
+      <c r="QE57" s="0"/>
+      <c r="QF57" s="0"/>
+      <c r="QG57" s="0"/>
+      <c r="QH57" s="0"/>
+      <c r="QI57" s="0"/>
+      <c r="QJ57" s="0"/>
+      <c r="QK57" s="0"/>
+      <c r="QL57" s="0"/>
+      <c r="QM57" s="0"/>
+      <c r="QN57" s="0"/>
+      <c r="QO57" s="0"/>
+      <c r="QP57" s="0"/>
+      <c r="QQ57" s="0"/>
+      <c r="QR57" s="0"/>
+      <c r="QS57" s="0"/>
+      <c r="QT57" s="0"/>
+      <c r="QU57" s="0"/>
+      <c r="QV57" s="0"/>
+      <c r="QW57" s="0"/>
+      <c r="QX57" s="0"/>
+      <c r="QY57" s="0"/>
+      <c r="QZ57" s="0"/>
+      <c r="RA57" s="0"/>
+      <c r="RB57" s="0"/>
+      <c r="RC57" s="0"/>
+      <c r="RD57" s="0"/>
+      <c r="RE57" s="0"/>
+      <c r="RF57" s="0"/>
+      <c r="RG57" s="0"/>
+      <c r="RH57" s="0"/>
+      <c r="RI57" s="0"/>
+      <c r="RJ57" s="0"/>
+      <c r="RK57" s="0"/>
+      <c r="RL57" s="0"/>
+      <c r="RM57" s="0"/>
+      <c r="RN57" s="0"/>
+      <c r="RO57" s="0"/>
+      <c r="RP57" s="0"/>
+      <c r="RQ57" s="0"/>
+      <c r="RR57" s="0"/>
+      <c r="RS57" s="0"/>
+      <c r="RT57" s="0"/>
+      <c r="RU57" s="0"/>
+      <c r="RV57" s="0"/>
+      <c r="RW57" s="0"/>
+      <c r="RX57" s="0"/>
+      <c r="RY57" s="0"/>
+      <c r="RZ57" s="0"/>
+      <c r="SA57" s="0"/>
+      <c r="SB57" s="0"/>
+      <c r="SC57" s="0"/>
+      <c r="SD57" s="0"/>
+      <c r="SE57" s="0"/>
+      <c r="SF57" s="0"/>
+      <c r="SG57" s="0"/>
+      <c r="SH57" s="0"/>
+      <c r="SI57" s="0"/>
+      <c r="SJ57" s="0"/>
+      <c r="SK57" s="0"/>
+      <c r="SL57" s="0"/>
+      <c r="SM57" s="0"/>
+      <c r="SN57" s="0"/>
+      <c r="SO57" s="0"/>
+      <c r="SP57" s="0"/>
+      <c r="SQ57" s="0"/>
+      <c r="SR57" s="0"/>
+      <c r="SS57" s="0"/>
+      <c r="ST57" s="0"/>
+      <c r="SU57" s="0"/>
+      <c r="SV57" s="0"/>
+      <c r="SW57" s="0"/>
+      <c r="SX57" s="0"/>
+      <c r="SY57" s="0"/>
+      <c r="SZ57" s="0"/>
+      <c r="TA57" s="0"/>
+      <c r="TB57" s="0"/>
+      <c r="TC57" s="0"/>
+      <c r="TD57" s="0"/>
+      <c r="TE57" s="0"/>
+      <c r="TF57" s="0"/>
+      <c r="TG57" s="0"/>
+      <c r="TH57" s="0"/>
+      <c r="TI57" s="0"/>
+      <c r="TJ57" s="0"/>
+      <c r="TK57" s="0"/>
+      <c r="TL57" s="0"/>
+      <c r="TM57" s="0"/>
+      <c r="TN57" s="0"/>
+      <c r="TO57" s="0"/>
+      <c r="TP57" s="0"/>
+      <c r="TQ57" s="0"/>
+      <c r="TR57" s="0"/>
+      <c r="TS57" s="0"/>
+      <c r="TT57" s="0"/>
+      <c r="TU57" s="0"/>
+      <c r="TV57" s="0"/>
+      <c r="TW57" s="0"/>
+      <c r="TX57" s="0"/>
+      <c r="TY57" s="0"/>
+      <c r="TZ57" s="0"/>
+      <c r="UA57" s="0"/>
+      <c r="UB57" s="0"/>
+      <c r="UC57" s="0"/>
+      <c r="UD57" s="0"/>
+      <c r="UE57" s="0"/>
+      <c r="UF57" s="0"/>
+      <c r="UG57" s="0"/>
+      <c r="UH57" s="0"/>
+      <c r="UI57" s="0"/>
+      <c r="UJ57" s="0"/>
+      <c r="UK57" s="0"/>
+      <c r="UL57" s="0"/>
+      <c r="UM57" s="0"/>
+      <c r="UN57" s="0"/>
+      <c r="UO57" s="0"/>
+      <c r="UP57" s="0"/>
+      <c r="UQ57" s="0"/>
+      <c r="UR57" s="0"/>
+      <c r="US57" s="0"/>
+      <c r="UT57" s="0"/>
+      <c r="UU57" s="0"/>
+      <c r="UV57" s="0"/>
+      <c r="UW57" s="0"/>
+      <c r="UX57" s="0"/>
+      <c r="UY57" s="0"/>
+      <c r="UZ57" s="0"/>
+      <c r="VA57" s="0"/>
+      <c r="VB57" s="0"/>
+      <c r="VC57" s="0"/>
+      <c r="VD57" s="0"/>
+      <c r="VE57" s="0"/>
+      <c r="VF57" s="0"/>
+      <c r="VG57" s="0"/>
+      <c r="VH57" s="0"/>
+      <c r="VI57" s="0"/>
+      <c r="VJ57" s="0"/>
+      <c r="VK57" s="0"/>
+      <c r="VL57" s="0"/>
+      <c r="VM57" s="0"/>
+      <c r="VN57" s="0"/>
+      <c r="VO57" s="0"/>
+      <c r="VP57" s="0"/>
+      <c r="VQ57" s="0"/>
+      <c r="VR57" s="0"/>
+      <c r="VS57" s="0"/>
+      <c r="VT57" s="0"/>
+      <c r="VU57" s="0"/>
+      <c r="VV57" s="0"/>
+      <c r="VW57" s="0"/>
+      <c r="VX57" s="0"/>
+      <c r="VY57" s="0"/>
+      <c r="VZ57" s="0"/>
+      <c r="WA57" s="0"/>
+      <c r="WB57" s="0"/>
+      <c r="WC57" s="0"/>
+      <c r="WD57" s="0"/>
+      <c r="WE57" s="0"/>
+      <c r="WF57" s="0"/>
+      <c r="WG57" s="0"/>
+      <c r="WH57" s="0"/>
+      <c r="WI57" s="0"/>
+      <c r="WJ57" s="0"/>
+      <c r="WK57" s="0"/>
+      <c r="WL57" s="0"/>
+      <c r="WM57" s="0"/>
+      <c r="WN57" s="0"/>
+      <c r="WO57" s="0"/>
+      <c r="WP57" s="0"/>
+      <c r="WQ57" s="0"/>
+      <c r="WR57" s="0"/>
+      <c r="WS57" s="0"/>
+      <c r="WT57" s="0"/>
+      <c r="WU57" s="0"/>
+      <c r="WV57" s="0"/>
+      <c r="WW57" s="0"/>
+      <c r="WX57" s="0"/>
+      <c r="WY57" s="0"/>
+      <c r="WZ57" s="0"/>
+      <c r="XA57" s="0"/>
+      <c r="XB57" s="0"/>
+      <c r="XC57" s="0"/>
+      <c r="XD57" s="0"/>
+      <c r="XE57" s="0"/>
+      <c r="XF57" s="0"/>
+      <c r="XG57" s="0"/>
+      <c r="XH57" s="0"/>
+      <c r="XI57" s="0"/>
+      <c r="XJ57" s="0"/>
+      <c r="XK57" s="0"/>
+      <c r="XL57" s="0"/>
+      <c r="XM57" s="0"/>
+      <c r="XN57" s="0"/>
+      <c r="XO57" s="0"/>
+      <c r="XP57" s="0"/>
+      <c r="XQ57" s="0"/>
+      <c r="XR57" s="0"/>
+      <c r="XS57" s="0"/>
+      <c r="XT57" s="0"/>
+      <c r="XU57" s="0"/>
+      <c r="XV57" s="0"/>
+      <c r="XW57" s="0"/>
+      <c r="XX57" s="0"/>
+      <c r="XY57" s="0"/>
+      <c r="XZ57" s="0"/>
+      <c r="YA57" s="0"/>
+      <c r="YB57" s="0"/>
+      <c r="YC57" s="0"/>
+      <c r="YD57" s="0"/>
+      <c r="YE57" s="0"/>
+      <c r="YF57" s="0"/>
+      <c r="YG57" s="0"/>
+      <c r="YH57" s="0"/>
+      <c r="YI57" s="0"/>
+      <c r="YJ57" s="0"/>
+      <c r="YK57" s="0"/>
+      <c r="YL57" s="0"/>
+      <c r="YM57" s="0"/>
+      <c r="YN57" s="0"/>
+      <c r="YO57" s="0"/>
+      <c r="YP57" s="0"/>
+      <c r="YQ57" s="0"/>
+      <c r="YR57" s="0"/>
+      <c r="YS57" s="0"/>
+      <c r="YT57" s="0"/>
+      <c r="YU57" s="0"/>
+      <c r="YV57" s="0"/>
+      <c r="YW57" s="0"/>
+      <c r="YX57" s="0"/>
+      <c r="YY57" s="0"/>
+      <c r="YZ57" s="0"/>
+      <c r="ZA57" s="0"/>
+      <c r="ZB57" s="0"/>
+      <c r="ZC57" s="0"/>
+      <c r="ZD57" s="0"/>
+      <c r="ZE57" s="0"/>
+      <c r="ZF57" s="0"/>
+      <c r="ZG57" s="0"/>
+      <c r="ZH57" s="0"/>
+      <c r="ZI57" s="0"/>
+      <c r="ZJ57" s="0"/>
+      <c r="ZK57" s="0"/>
+      <c r="ZL57" s="0"/>
+      <c r="ZM57" s="0"/>
+      <c r="ZN57" s="0"/>
+      <c r="ZO57" s="0"/>
+      <c r="ZP57" s="0"/>
+      <c r="ZQ57" s="0"/>
+      <c r="ZR57" s="0"/>
+      <c r="ZS57" s="0"/>
+      <c r="ZT57" s="0"/>
+      <c r="ZU57" s="0"/>
+      <c r="ZV57" s="0"/>
+      <c r="ZW57" s="0"/>
+      <c r="ZX57" s="0"/>
+      <c r="ZY57" s="0"/>
+      <c r="ZZ57" s="0"/>
+      <c r="AAA57" s="0"/>
+      <c r="AAB57" s="0"/>
+      <c r="AAC57" s="0"/>
+      <c r="AAD57" s="0"/>
+      <c r="AAE57" s="0"/>
+      <c r="AAF57" s="0"/>
+      <c r="AAG57" s="0"/>
+      <c r="AAH57" s="0"/>
+      <c r="AAI57" s="0"/>
+      <c r="AAJ57" s="0"/>
+      <c r="AAK57" s="0"/>
+      <c r="AAL57" s="0"/>
+      <c r="AAM57" s="0"/>
+      <c r="AAN57" s="0"/>
+      <c r="AAO57" s="0"/>
+      <c r="AAP57" s="0"/>
+      <c r="AAQ57" s="0"/>
+      <c r="AAR57" s="0"/>
+      <c r="AAS57" s="0"/>
+      <c r="AAT57" s="0"/>
+      <c r="AAU57" s="0"/>
+      <c r="AAV57" s="0"/>
+      <c r="AAW57" s="0"/>
+      <c r="AAX57" s="0"/>
+      <c r="AAY57" s="0"/>
+      <c r="AAZ57" s="0"/>
+      <c r="ABA57" s="0"/>
+      <c r="ABB57" s="0"/>
+      <c r="ABC57" s="0"/>
+      <c r="ABD57" s="0"/>
+      <c r="ABE57" s="0"/>
+      <c r="ABF57" s="0"/>
+      <c r="ABG57" s="0"/>
+      <c r="ABH57" s="0"/>
+      <c r="ABI57" s="0"/>
+      <c r="ABJ57" s="0"/>
+      <c r="ABK57" s="0"/>
+      <c r="ABL57" s="0"/>
+      <c r="ABM57" s="0"/>
+      <c r="ABN57" s="0"/>
+      <c r="ABO57" s="0"/>
+      <c r="ABP57" s="0"/>
+      <c r="ABQ57" s="0"/>
+      <c r="ABR57" s="0"/>
+      <c r="ABS57" s="0"/>
+      <c r="ABT57" s="0"/>
+      <c r="ABU57" s="0"/>
+      <c r="ABV57" s="0"/>
+      <c r="ABW57" s="0"/>
+      <c r="ABX57" s="0"/>
+      <c r="ABY57" s="0"/>
+      <c r="ABZ57" s="0"/>
+      <c r="ACA57" s="0"/>
+      <c r="ACB57" s="0"/>
+      <c r="ACC57" s="0"/>
+      <c r="ACD57" s="0"/>
+      <c r="ACE57" s="0"/>
+      <c r="ACF57" s="0"/>
+      <c r="ACG57" s="0"/>
+      <c r="ACH57" s="0"/>
+      <c r="ACI57" s="0"/>
+      <c r="ACJ57" s="0"/>
+      <c r="ACK57" s="0"/>
+      <c r="ACL57" s="0"/>
+      <c r="ACM57" s="0"/>
+      <c r="ACN57" s="0"/>
+      <c r="ACO57" s="0"/>
+      <c r="ACP57" s="0"/>
+      <c r="ACQ57" s="0"/>
+      <c r="ACR57" s="0"/>
+      <c r="ACS57" s="0"/>
+      <c r="ACT57" s="0"/>
+      <c r="ACU57" s="0"/>
+      <c r="ACV57" s="0"/>
+      <c r="ACW57" s="0"/>
+      <c r="ACX57" s="0"/>
+      <c r="ACY57" s="0"/>
+      <c r="ACZ57" s="0"/>
+      <c r="ADA57" s="0"/>
+      <c r="ADB57" s="0"/>
+      <c r="ADC57" s="0"/>
+      <c r="ADD57" s="0"/>
+      <c r="ADE57" s="0"/>
+      <c r="ADF57" s="0"/>
+      <c r="ADG57" s="0"/>
+      <c r="ADH57" s="0"/>
+      <c r="ADI57" s="0"/>
+      <c r="ADJ57" s="0"/>
+      <c r="ADK57" s="0"/>
+      <c r="ADL57" s="0"/>
+      <c r="ADM57" s="0"/>
+      <c r="ADN57" s="0"/>
+      <c r="ADO57" s="0"/>
+      <c r="ADP57" s="0"/>
+      <c r="ADQ57" s="0"/>
+      <c r="ADR57" s="0"/>
+      <c r="ADS57" s="0"/>
+      <c r="ADT57" s="0"/>
+      <c r="ADU57" s="0"/>
+      <c r="ADV57" s="0"/>
+      <c r="ADW57" s="0"/>
+      <c r="ADX57" s="0"/>
+      <c r="ADY57" s="0"/>
+      <c r="ADZ57" s="0"/>
+      <c r="AEA57" s="0"/>
+      <c r="AEB57" s="0"/>
+      <c r="AEC57" s="0"/>
+      <c r="AED57" s="0"/>
+      <c r="AEE57" s="0"/>
+      <c r="AEF57" s="0"/>
+      <c r="AEG57" s="0"/>
+      <c r="AEH57" s="0"/>
+      <c r="AEI57" s="0"/>
+      <c r="AEJ57" s="0"/>
+      <c r="AEK57" s="0"/>
+      <c r="AEL57" s="0"/>
+      <c r="AEM57" s="0"/>
+      <c r="AEN57" s="0"/>
+      <c r="AEO57" s="0"/>
+      <c r="AEP57" s="0"/>
+      <c r="AEQ57" s="0"/>
+      <c r="AER57" s="0"/>
+      <c r="AES57" s="0"/>
+      <c r="AET57" s="0"/>
+      <c r="AEU57" s="0"/>
+      <c r="AEV57" s="0"/>
+      <c r="AEW57" s="0"/>
+      <c r="AEX57" s="0"/>
+      <c r="AEY57" s="0"/>
+      <c r="AEZ57" s="0"/>
+      <c r="AFA57" s="0"/>
+      <c r="AFB57" s="0"/>
+      <c r="AFC57" s="0"/>
+      <c r="AFD57" s="0"/>
+      <c r="AFE57" s="0"/>
+      <c r="AFF57" s="0"/>
+      <c r="AFG57" s="0"/>
+      <c r="AFH57" s="0"/>
+      <c r="AFI57" s="0"/>
+      <c r="AFJ57" s="0"/>
+      <c r="AFK57" s="0"/>
+      <c r="AFL57" s="0"/>
+      <c r="AFM57" s="0"/>
+      <c r="AFN57" s="0"/>
+      <c r="AFO57" s="0"/>
+      <c r="AFP57" s="0"/>
+      <c r="AFQ57" s="0"/>
+      <c r="AFR57" s="0"/>
+      <c r="AFS57" s="0"/>
+      <c r="AFT57" s="0"/>
+      <c r="AFU57" s="0"/>
+      <c r="AFV57" s="0"/>
+      <c r="AFW57" s="0"/>
+      <c r="AFX57" s="0"/>
+      <c r="AFY57" s="0"/>
+      <c r="AFZ57" s="0"/>
+      <c r="AGA57" s="0"/>
+      <c r="AGB57" s="0"/>
+      <c r="AGC57" s="0"/>
+      <c r="AGD57" s="0"/>
+      <c r="AGE57" s="0"/>
+      <c r="AGF57" s="0"/>
+      <c r="AGG57" s="0"/>
+      <c r="AGH57" s="0"/>
+      <c r="AGI57" s="0"/>
+      <c r="AGJ57" s="0"/>
+      <c r="AGK57" s="0"/>
+      <c r="AGL57" s="0"/>
+      <c r="AGM57" s="0"/>
+      <c r="AGN57" s="0"/>
+      <c r="AGO57" s="0"/>
+      <c r="AGP57" s="0"/>
+      <c r="AGQ57" s="0"/>
+      <c r="AGR57" s="0"/>
+      <c r="AGS57" s="0"/>
+      <c r="AGT57" s="0"/>
+      <c r="AGU57" s="0"/>
+      <c r="AGV57" s="0"/>
+      <c r="AGW57" s="0"/>
+      <c r="AGX57" s="0"/>
+      <c r="AGY57" s="0"/>
+      <c r="AGZ57" s="0"/>
+      <c r="AHA57" s="0"/>
+      <c r="AHB57" s="0"/>
+      <c r="AHC57" s="0"/>
+      <c r="AHD57" s="0"/>
+      <c r="AHE57" s="0"/>
+      <c r="AHF57" s="0"/>
+      <c r="AHG57" s="0"/>
+      <c r="AHH57" s="0"/>
+      <c r="AHI57" s="0"/>
+      <c r="AHJ57" s="0"/>
+      <c r="AHK57" s="0"/>
+      <c r="AHL57" s="0"/>
+      <c r="AHM57" s="0"/>
+      <c r="AHN57" s="0"/>
+      <c r="AHO57" s="0"/>
+      <c r="AHP57" s="0"/>
+      <c r="AHQ57" s="0"/>
+      <c r="AHR57" s="0"/>
+      <c r="AHS57" s="0"/>
+      <c r="AHT57" s="0"/>
+      <c r="AHU57" s="0"/>
+      <c r="AHV57" s="0"/>
+      <c r="AHW57" s="0"/>
+      <c r="AHX57" s="0"/>
+      <c r="AHY57" s="0"/>
+      <c r="AHZ57" s="0"/>
+      <c r="AIA57" s="0"/>
+      <c r="AIB57" s="0"/>
+      <c r="AIC57" s="0"/>
+      <c r="AID57" s="0"/>
+      <c r="AIE57" s="0"/>
+      <c r="AIF57" s="0"/>
+      <c r="AIG57" s="0"/>
+      <c r="AIH57" s="0"/>
+      <c r="AII57" s="0"/>
+      <c r="AIJ57" s="0"/>
+      <c r="AIK57" s="0"/>
+      <c r="AIL57" s="0"/>
+      <c r="AIM57" s="0"/>
+      <c r="AIN57" s="0"/>
+      <c r="AIO57" s="0"/>
+      <c r="AIP57" s="0"/>
+      <c r="AIQ57" s="0"/>
+      <c r="AIR57" s="0"/>
+      <c r="AIS57" s="0"/>
+      <c r="AIT57" s="0"/>
+      <c r="AIU57" s="0"/>
+      <c r="AIV57" s="0"/>
+      <c r="AIW57" s="0"/>
+      <c r="AIX57" s="0"/>
+      <c r="AIY57" s="0"/>
+      <c r="AIZ57" s="0"/>
+      <c r="AJA57" s="0"/>
+      <c r="AJB57" s="0"/>
+      <c r="AJC57" s="0"/>
+      <c r="AJD57" s="0"/>
+      <c r="AJE57" s="0"/>
+      <c r="AJF57" s="0"/>
+      <c r="AJG57" s="0"/>
+      <c r="AJH57" s="0"/>
+      <c r="AJI57" s="0"/>
+      <c r="AJJ57" s="0"/>
+      <c r="AJK57" s="0"/>
+      <c r="AJL57" s="0"/>
+      <c r="AJM57" s="0"/>
+      <c r="AJN57" s="0"/>
+      <c r="AJO57" s="0"/>
+      <c r="AJP57" s="0"/>
+      <c r="AJQ57" s="0"/>
+      <c r="AJR57" s="0"/>
+      <c r="AJS57" s="0"/>
+      <c r="AJT57" s="0"/>
+      <c r="AJU57" s="0"/>
+      <c r="AJV57" s="0"/>
+      <c r="AJW57" s="0"/>
+      <c r="AJX57" s="0"/>
+      <c r="AJY57" s="0"/>
+      <c r="AJZ57" s="0"/>
+      <c r="AKA57" s="0"/>
+      <c r="AKB57" s="0"/>
+      <c r="AKC57" s="0"/>
+      <c r="AKD57" s="0"/>
+      <c r="AKE57" s="0"/>
+      <c r="AKF57" s="0"/>
+      <c r="AKG57" s="0"/>
+      <c r="AKH57" s="0"/>
+      <c r="AKI57" s="0"/>
+      <c r="AKJ57" s="0"/>
+      <c r="AKK57" s="0"/>
+      <c r="AKL57" s="0"/>
+      <c r="AKM57" s="0"/>
+      <c r="AKN57" s="0"/>
+      <c r="AKO57" s="0"/>
+      <c r="AKP57" s="0"/>
+      <c r="AKQ57" s="0"/>
+      <c r="AKR57" s="0"/>
+      <c r="AKS57" s="0"/>
+      <c r="AKT57" s="0"/>
+      <c r="AKU57" s="0"/>
+      <c r="AKV57" s="0"/>
+      <c r="AKW57" s="0"/>
+      <c r="AKX57" s="0"/>
+      <c r="AKY57" s="0"/>
+      <c r="AKZ57" s="0"/>
+      <c r="ALA57" s="0"/>
+      <c r="ALB57" s="0"/>
+      <c r="ALC57" s="0"/>
+      <c r="ALD57" s="0"/>
+      <c r="ALE57" s="0"/>
+      <c r="ALF57" s="0"/>
+      <c r="ALG57" s="0"/>
+      <c r="ALH57" s="0"/>
+      <c r="ALI57" s="0"/>
+      <c r="ALJ57" s="0"/>
+      <c r="ALK57" s="0"/>
+      <c r="ALL57" s="0"/>
+      <c r="ALM57" s="0"/>
+      <c r="ALN57" s="0"/>
+      <c r="ALO57" s="0"/>
+      <c r="ALP57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C62" s="1" t="s">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C61" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="C63" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C68" s="1" t="s">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="C69" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C75" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C76" s="1" t="s">
+    <row r="74" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C74" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C78" s="1" t="s">
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C77" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C79" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>86</v>
       </c>
     </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C80" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="C82" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C83" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
begin media cloud downloading
</commit_message>
<xml_diff>
--- a/_bots/gorkathebot/gorkathebot.xlsx
+++ b/_bots/gorkathebot/gorkathebot.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">VERSION</t>
   </si>
   <si>
-    <t xml:space="preserve">0.2.12</t>
+    <t xml:space="preserve">0.2.13</t>
   </si>
   <si>
     <t xml:space="preserve">gorkathebot</t>
@@ -205,7 +205,7 @@
     <t xml:space="preserve">photoEli</t>
   </si>
   <si>
-    <t xml:space="preserve">eli_{number}.jpg</t>
+    <t xml:space="preserve">firsts/eli_{number}.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">filenameUploaded</t>

</xml_diff>

<commit_message>
begin mm support for all media types
</commit_message>
<xml_diff>
--- a/_bots/gorkathebot/gorkathebot.xlsx
+++ b/_bots/gorkathebot/gorkathebot.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="184">
   <si>
     <t xml:space="preserve">BOTBASIC</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">VERSION</t>
   </si>
   <si>
-    <t xml:space="preserve">0.2.14</t>
+    <t xml:space="preserve">0.2.16</t>
   </si>
   <si>
     <t xml:space="preserve">gorkathebot</t>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">commandOptions</t>
   </si>
   <si>
-    <t xml:space="preserve">Choose /ai /test</t>
+    <t xml:space="preserve">Choose /ai /pixels /test</t>
   </si>
   <si>
     <t xml:space="preserve">sendAnImage</t>
@@ -244,6 +244,42 @@
     <t xml:space="preserve">Image format is {format}</t>
   </si>
   <si>
+    <t xml:space="preserve">whatWasThis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What was this?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wasAI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artificial Inteligence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wasAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artificial Stupidity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wasBoth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thanks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">totalPixels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image is {width} pixels wide and {height} pixels tall and has {pixels} pixels</t>
+  </si>
+  <si>
     <t xml:space="preserve">MENUS</t>
   </si>
   <si>
@@ -349,6 +385,12 @@
     <t xml:space="preserve">PRINT myage</t>
   </si>
   <si>
+    <t xml:space="preserve">MENU TITLE whatWasThis OPTIONS wasAI wasAS wasBoth TO wasThis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINT thanks</t>
+  </si>
+  <si>
     <t xml:space="preserve">GOTO menu</t>
   </si>
   <si>
@@ -391,6 +433,30 @@
     <t xml:space="preserve">SET tryToLaugh absurd1</t>
   </si>
   <si>
+    <t xml:space="preserve">/pixels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INPUT image TITLE sendOnlyPhoto TO id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTRACT width FROM id TO width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTRACT height FROM id TO height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET pixels width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUL pixels height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINT totalPixels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOTO start</t>
+  </si>
+  <si>
     <t xml:space="preserve">/test</t>
   </si>
   <si>
@@ -418,9 +484,6 @@
     <t xml:space="preserve">CLEAR id</t>
   </si>
   <si>
-    <t xml:space="preserve">INPUT image TITLE sendOnlyPhoto TO id</t>
-  </si>
-  <si>
     <t xml:space="preserve">PRINT mediaId1</t>
   </si>
   <si>
@@ -499,7 +562,7 @@
     <t xml:space="preserve">/imagenumber</t>
   </si>
   <si>
-    <t xml:space="preserve">INPUT integer TITLE imageNumber TO number</t>
+    <t xml:space="preserve">MENU TITLE imageNumber OPTIONS 1 2 3 4 5 6 7 8 9 10 TO number</t>
   </si>
   <si>
     <t xml:space="preserve">sendEli2</t>
@@ -717,7 +780,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P153"/>
+  <dimension ref="A1:P169"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
@@ -1082,598 +1145,696 @@
       </c>
     </row>
     <row r="43" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7"/>
-    </row>
-    <row r="44" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="s">
+      <c r="A43" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-      <c r="P46" s="5"/>
+      <c r="C43" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="47" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="7"/>
+    </row>
+    <row r="50" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="5"/>
+    </row>
+    <row r="53" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="48" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
-      <c r="P51" s="5"/>
-    </row>
-    <row r="52" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C53" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="54" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="55" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="5"/>
-      <c r="M56" s="4"/>
-      <c r="N56" s="4"/>
-      <c r="O56" s="4"/>
-      <c r="P56" s="5"/>
-    </row>
-    <row r="57" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
+    <row r="56" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="5"/>
+    </row>
+    <row r="58" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="60" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="61" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E61" s="1" t="s">
+    </row>
+    <row r="59" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="5"/>
+    </row>
+    <row r="63" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F63" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="62" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="G63" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="64" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="5"/>
-      <c r="M65" s="4"/>
-      <c r="N65" s="4"/>
-      <c r="O65" s="4"/>
-      <c r="P65" s="5"/>
+    <row r="65" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="66" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="67" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>96</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="67" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="68" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="69" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="71" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C71" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="72" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="74" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C74" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
+    <row r="70" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+      <c r="O71" s="4"/>
+      <c r="P71" s="5"/>
+    </row>
+    <row r="72" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="75" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="76" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="77" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C78" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="78" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="C79" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="B82" s="1" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="1" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C89" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="1" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C94" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="C96" s="1" t="s">
-        <v>118</v>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C97" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="C98" s="1" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="1" t="s">
-        <v>118</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C100" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="C101" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C102" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="C104" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C105" s="1" t="s">
-        <v>94</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="C107" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C108" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="C109" s="1" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="1" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0"/>
       <c r="C113" s="1" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C114" s="1" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C115" s="1" t="s">
-        <v>134</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C116" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="C117" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C118" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C119" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>146</v>
+      </c>
       <c r="C120" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>140</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C121" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="s">
+        <v>148</v>
+      </c>
       <c r="C123" s="1" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C124" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C125" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C126" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C127" s="1" t="s">
-        <v>145</v>
+        <v>106</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="C128" s="1" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0"/>
       <c r="C129" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C130" s="1" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C132" s="1" t="s">
-        <v>131</v>
+      <c r="C131" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="C133" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C134" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C135" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C136" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C137" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="C138" s="1" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B139" s="1" t="s">
-        <v>153</v>
+      <c r="C139" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C140" s="1" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C141" s="1" t="s">
-        <v>118</v>
+        <v>164</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B142" s="1" t="s">
-        <v>155</v>
+      <c r="C142" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C143" s="1" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C144" s="1" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C145" s="1" t="s">
-        <v>118</v>
+        <v>168</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="s">
-        <v>158</v>
+      <c r="C146" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C147" s="1" t="s">
-        <v>159</v>
-      </c>
+      <c r="A147" s="0"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="1" t="s">
+        <v>169</v>
+      </c>
       <c r="C148" s="1" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B149" s="1" t="s">
-        <v>160</v>
+      <c r="C149" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C150" s="1" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C151" s="1" t="s">
-        <v>133</v>
+        <v>172</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C152" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C153" s="1" t="s">
-        <v>134</v>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C154" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B155" s="0"/>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B156" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C157" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B159" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C160" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C161" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0"/>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C164" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B165" s="0"/>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B166" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C167" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C168" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C169" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish receiving and sending different media types
</commit_message>
<xml_diff>
--- a/_bots/gorkathebot/gorkathebot.xlsx
+++ b/_bots/gorkathebot/gorkathebot.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">VERSION</t>
   </si>
   <si>
-    <t xml:space="preserve">0.2.19</t>
+    <t xml:space="preserve">0.2.20</t>
   </si>
   <si>
     <t xml:space="preserve">gorkathebot</t>
@@ -661,7 +661,7 @@
     <t xml:space="preserve">/sendmedia</t>
   </si>
   <si>
-    <t xml:space="preserve">OPTIONS oAUdio oDocument oImage oVideo oVideonote oVoice</t>
+    <t xml:space="preserve">OPTIONS oAudio oDocument oImage oVideo oVideonote oVoice</t>
   </si>
   <si>
     <t xml:space="preserve">MENU TITLE selectMediaType TO option</t>
@@ -936,7 +936,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
allow underscores in identifiers
</commit_message>
<xml_diff>
--- a/_bots/gorkathebot/gorkathebot.xlsx
+++ b/_bots/gorkathebot/gorkathebot.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="483">
   <si>
     <t xml:space="preserve">BOTBASIC</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">VERSION</t>
   </si>
   <si>
-    <t xml:space="preserve">0.2.28</t>
+    <t xml:space="preserve">0.3.1</t>
   </si>
   <si>
     <t xml:space="preserve">gorkathebot</t>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">es</t>
+    <t xml:space="preserve">en</t>
   </si>
   <si>
     <t xml:space="preserve">myname</t>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">commandOptions</t>
   </si>
   <si>
-    <t xml:space="preserve">Choose /ai /pixels /test</t>
+    <t xml:space="preserve">Choose /ai /pixels /test /svitolina</t>
   </si>
   <si>
     <t xml:space="preserve">sendMedia</t>
@@ -382,6 +382,327 @@
     <t xml:space="preserve">This is the antipodeans:</t>
   </si>
   <si>
+    <t xml:space="preserve">rem_svb_section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">svitolinabot vars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rem_svb_videos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img_18brisbane_d2_hl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20180101_day2_hl_elina_vs_carla-suarez-navarro_480p.m4v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img_18brisbane_d2_sotd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20180101_day2_sotd_elina_vs_carla-suarez-navarro_480p.m4v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img_18brisbane_d3_hl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20180103_day3_hl_elina_vs_ana-konjuh_480p.m4v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img_18brisbane_d4qf_hl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20180104_day4qf_hl_elina_vs_johanna-konta_480p.m4v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img_18brisbane_d5sf_hl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20180105_day5sf_hl_elina_vs_karolina-pliskova_480p.m4v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img_18brisbane_d5sf_sotd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20180105_day5sf_sotd_elina_vs_karolina-pliskova_480p.m4v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img_18brisbane_d6f_hl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20180106_day6f_hl_elina_vs_aliaksandra-sasnovic_480p.m4v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rem_svb_images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rem_svb_images_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rem svb_genericstrings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prmMediatype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Want to see…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optVideos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Videos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optImages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optSotd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shots of the day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optQuotes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quotes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prmDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optDay1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optDay2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optDay3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optDay4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optDay5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optDay6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optDay7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optChooseOne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose one…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optHighlighs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Highlights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optQuote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elina’s words</t>
+  </si>
+  <si>
+    <t xml:space="preserve">txtElina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">txtEli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">txtElinaS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elina Svitolina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">txtSvitolina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Svitolina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">txtThanks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prmAgain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Want to see again?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optYes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">txtByeByEli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">txtWaitForVideo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wait while video downloads…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">txtQuote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">___{quote}___</t>
+  </si>
+  <si>
+    <t xml:space="preserve">txtFromLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: {link}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rem_svb_prompts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prmHi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi, I’m Eli, and this is my bot ;-)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prmTournament</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose a tournament</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opt18brisbane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brisbane 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">txtWasAbye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{eliname} didn’t play this day because of a bye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rem_svb_quotes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qte_18brisbane_d2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"I always like to come here. I like the audience, I like the performance on this court, for me it's always a special feeling, because before I had heavy matches in Brisbane, every time I go out on the court, it's always loaded on the game."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qte_18brisbane_d2_lnk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://vk.com/@svitolina-elina-svitolina-s-kontoi-nam-predstoit-esche-odna-bitva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qte_18brisbane_d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"It's always unpleasant to get injured, especially when it happens during the match and I hope that Johanna will be able to recover quickly and we'll see her on the court soon. She's a very good player and played a great match today. After the first set I lost, I told myself that you need to fight for every ball to the end and wait for your chances."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qte_18brisbane_d4_lnk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://svitolina.com/ru/news/456-news-04-01.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qte_18brisbane_d5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"In such matches it's important to be very focused and wait for your small chances. So, I knew that in the second set I needed to be as collected as possible, good to serve and be ready for these moments. I had a good tiebreak, played it at 100%."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qte_18brisbane_d5_lnk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://vk.com/@svitolina-elina-svitolina-taibreik-vo-vtorom-sete-ya-otygrala-na-vse-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qte_18brisbane_d6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Good evening to everyone! It's very nice to see the whole stadium. It's incredible to start the new year with the title. I had a difficult offseason, like everyone else, so opening the season with a victory in the tournament is always something very, very special."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qte_18brisbane_d6_lnk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://vk.com/@svitolina-elina-svitolina-otkryvat-sezon-pobedoi-na-turnire-eto-vseg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qte_18brisbane_d7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"I did not have so much time to recover from the semifinals, I slept very, very badly, I hope you did not notice it, because I tried ... I hope, I'm a good actress. I tried to be really focused on what I should do on the court, and it was very important for me to focus on my game plan, and everything worked very well, of course, you can see it on the scoreboard."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qte_18brisbane_d7_lnk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://vk.com/@svitolina-elina-svitolina-nadeus-ya-horoshaya-aktrisa-i-vy-ne-zametili</t>
+  </si>
+  <si>
     <t xml:space="preserve">MENUS</t>
   </si>
   <si>
@@ -683,6 +1004,120 @@
   </si>
   <si>
     <t xml:space="preserve">MENU TITLE selectMediaType TO option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ option oAudio THEN BLOAD mediaAudio1 AS audio TO id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ option oDocument THEN BLOAD mediaDocument1 AS document TO id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ option oImage THEN BLOAD mediaImage1 AS image TO id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ option oVideo THEN BLOAD mediaVideo1 AS video TO id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ option oVideonote THEN BLOAD mediaVideonote1 AS videonote TO id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ option oVoice THEN BLOAD mediaVoice1 AS voice TO id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EMPTY id THEN PRINT error : GOTO sm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/latlon /antipodeans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INPUT location TITLE enterLocation TO id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTRACT latitude FROM id TO lat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTRACT longitude FROM id TO lon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINT yourLocationIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINT oppositeLocation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUL lat -1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INC lon 180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUILD location SET longitude lon latitude lat TO id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REM svitolinabot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENTRYHOOK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOCALE en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/svitolinabot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">svitolinabot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINT prmHi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eli_menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION opt18brisbane GOSUB tt18brisbane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MENU TITLE prmTournament TO tournament</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINT txtThanks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MENU TITLE prmAgain OPTIONS optYes optNo TO way</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ way txtYes THEN GOTO eli_menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisbane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION optVideos GOSUB tt18brisVideos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REM OPTION optImages GOSUB tt18brisImages : REM TODO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION optSotd GOSUB tt18brisSotd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REM OPTION optQuotes GOSUB tt18brisQuotes : REM TODO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION optDay GOSUB tt18brisDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MENU TITLE prmMediaType TO way</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisVideos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION optDay1 GOSUB tt18brisVD1</t>
   </si>
   <si>
     <r>
@@ -692,7 +1127,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">IF EQ option oAudio THEN </t>
+      <t xml:space="preserve">OPTION </t>
     </r>
     <r>
       <rPr>
@@ -700,10 +1135,8 @@
         <rFont val="Liberation Sans Narrow"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">BLOAD mediaAudio1 AS audio TO id</t>
+      <t xml:space="preserve">optDay2 GOSUB </t>
     </r>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -711,7 +1144,18 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">IF EQ option oDocument THEN BLOAD </t>
+      <t xml:space="preserve">tt18brisVD2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">OPTION </t>
     </r>
     <r>
       <rPr>
@@ -719,53 +1163,512 @@
         <rFont val="Liberation Sans Narrow"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">mediaDocument1 AS document TO id</t>
+      <t xml:space="preserve">optDay3 GOSUB </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">IF EQ option oImage THEN BLOAD mediaImage1 AS image TO id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF EQ option oVideo THEN BLOAD mediaVideo1 AS video TO id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF EQ option oVideonote THEN BLOAD mediaVideonote1 AS videonote TO id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF EQ option oVoice THEN BLOAD mediaVoice1 AS voice TO id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF EMPTY id THEN PRINT error : GOTO sm1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sm1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/latlon /antipodeans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INPUT location TITLE enterLocation TO id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXTRACT latitude FROM id TO lat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXTRACT longitude FROM id TO lon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRINT yourLocationIs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRINT oppositeLocation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUL lat -1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INC lon 180</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUILD location SET longitude lon latitude lat TO id</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tt18brisVD3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">OPTION </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">optDay4 GOSUB </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tt18brisVD4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">OPTION </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">optDay5 GOSUB </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tt18brisVD5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">OPTION </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">optDay6 GOSUB </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tt18brisVD6</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">MENU TITLE prmDay TO way</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisDbye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB rotateName TO eliname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINT txtWasAbye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisVD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOTO tt18brisDbye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisVD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARGS day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day 2 THEN SET fn img_18brisbane_d2_hl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day 3 THEN SET fn img_18brisbane_d3_hl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day 4 THEN SET fn img_18brisbane_d4qf_hl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day 5 THEN SET fn img_18brisbane_d5sf_hl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day 6 THEN SET fn img_18brisbane_d6f_hl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day -2 THEN SET fn img_18brisbane_d2_sotd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day -5 THEN SET fn img_18brisbane_d5sf_sotd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisVD fn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisVD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARGS fn_filename</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET ffn fn_fullfilename18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLOAD ffn AS video TO id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINT txtWaitForVideo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisVD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisVD0 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisVD3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisVD0 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisVD4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisVD0 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisVD5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisVD0 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisVD6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisVD0 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisSotd</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">OPTION </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">optDay2 GOSUB </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tt18brisSD2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">OPTION </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">optDay5 GOSUB </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tt18brisSD5</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisSD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisVD0 -2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisSD5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisVD0 -5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION optDay1 GOSUB tt18brisD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION optDay2 GOSUB tt18brisD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION optDay3 GOSUB tt18brisD3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION optDay4 GOSUB tt18brisD4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION optDay5 GOSUB tt18brisD5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION optDay6 GOSUB tt18brisD6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MENU TITLE prmDay TO day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisDbye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB isThereContent day TO hl sotd quote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REM MENU OPTIONS optVideos optSotd optQuotes TITLE prmMediaType TO way</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MENU </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">TITLE prmMediaType </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">OPTIONS optHl optSotd TO way</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ way optHl THEN GOSUB tt18brisDHl day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ way optSotd THEN GOSUB tt18brisDSotd day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ way optQuotes THEN GOSUB tt18brisDQuotes day : REM to_do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisD 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisD3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisD 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisD4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisD 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisD5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisD 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisD6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisD 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisDHl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisVD0 day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisDSotd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MUL day -1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisQuotes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION optDay2 GOSUB tt18brisQ2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION optDay4 GOSUB tt18brisQ4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION optDay5 GOSUB tt18brisQ5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION optDay6 GOSUB tt18brisQ6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION optDay7 GOSUB tt18brisQ7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisQD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day 2 THEN SET qt qte_18brisbane_d2 : SET lnk qte_18brisbane_d2_lnk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day 4 THEN SET qt qte_18brisbane_d4 : SET lnk qte_18brisbane_d4_lnk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day 5 THEN SET qt qte_18brisbane_d5 : SET lnk qte_18brisbane_d5_lnk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day 6 THEN SET qt qte_18brisbane_d6 : SET lnk qte_18brisbane_d6_lnk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day 7 THEN SET qt qte_18brisbane_d2 : SET lnk qte_18brisbane_d7_lnk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisQD qt lnk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisQD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARGS quote link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINT txtQuote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINT txtFromLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisQ2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisQD0 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisQ4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisQD0 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisQ5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisQD0 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisQ6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisQD0 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tt18brisQ7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOSUB tt18brisQD0 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isThereContent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day 2 THEN SET hl 1 : SET sotd 0 : SET quote 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day 3 THEN SET hl 1 : SET sotd 1 : SET quote 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day 4 THEN SET hl 1 : SET sotd 0 : SET quote 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day 5 THEN SET hl 1 : SET sotd 1 : SET quote 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ day 6 THEN SET hl 1 : SET sotd 0 : SET quote 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RETURN hl sotd quote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotateName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EMPTY nameCounter THEN SET nameCounter 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INC nameCounter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF GT nameCounter 4 THEN SET nameCounter 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ nameCounter 1 THEN SET name txtElina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ nameCounter 2 THEN SET name txtEli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ nameCounter 3 THEN SET name txtSvitolina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF EQ nameCounter 4 THEN SET name txtElinaS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RETURN name</t>
   </si>
 </sst>
 </file>
@@ -775,7 +1678,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -806,6 +1709,13 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Liberation Sans Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Liberation Sans Narrow"/>
       <family val="2"/>
       <charset val="1"/>
@@ -974,14 +1884,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P209"/>
+  <dimension ref="A1:P446"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A350" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B383" activeCellId="0" sqref="B383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1331,7 +2237,7 @@
       </c>
     </row>
     <row r="42" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1339,7 +2245,7 @@
       </c>
     </row>
     <row r="43" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -1347,7 +2253,7 @@
       </c>
     </row>
     <row r="44" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1355,7 +2261,7 @@
       </c>
     </row>
     <row r="45" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -1363,7 +2269,7 @@
       </c>
     </row>
     <row r="46" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -1371,7 +2277,7 @@
       </c>
     </row>
     <row r="47" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="1" t="s">
         <v>82</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -1379,7 +2285,7 @@
       </c>
     </row>
     <row r="48" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -1387,7 +2293,7 @@
       </c>
     </row>
     <row r="49" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -1395,7 +2301,7 @@
       </c>
     </row>
     <row r="50" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -1403,7 +2309,7 @@
       </c>
     </row>
     <row r="51" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C51" s="1" t="s">
@@ -1411,7 +2317,7 @@
       </c>
     </row>
     <row r="52" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -1419,7 +2325,7 @@
       </c>
     </row>
     <row r="53" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -1427,7 +2333,7 @@
       </c>
     </row>
     <row r="54" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -1435,7 +2341,7 @@
       </c>
     </row>
     <row r="55" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -1443,7 +2349,7 @@
       </c>
     </row>
     <row r="56" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -1451,7 +2357,7 @@
       </c>
     </row>
     <row r="57" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -1459,7 +2365,7 @@
       </c>
     </row>
     <row r="58" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -1467,7 +2373,7 @@
       </c>
     </row>
     <row r="59" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C59" s="1" t="s">
@@ -1475,7 +2381,7 @@
       </c>
     </row>
     <row r="60" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -1483,7 +2389,7 @@
       </c>
     </row>
     <row r="61" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -1491,7 +2397,7 @@
       </c>
     </row>
     <row r="62" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C62" s="1" t="s">
@@ -1499,7 +2405,7 @@
       </c>
     </row>
     <row r="63" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -1507,7 +2413,7 @@
       </c>
     </row>
     <row r="64" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="1" t="s">
         <v>116</v>
       </c>
       <c r="C64" s="1" t="s">
@@ -1515,787 +2421,2036 @@
       </c>
     </row>
     <row r="65" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="7" t="s">
+      <c r="A65" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="66" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="7"/>
-    </row>
-    <row r="67" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="s">
+    <row r="66" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="4"/>
-      <c r="F69" s="4"/>
-      <c r="G69" s="4"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="4"/>
-      <c r="J69" s="4"/>
-      <c r="K69" s="4"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="4"/>
-      <c r="N69" s="4"/>
-      <c r="O69" s="4"/>
-      <c r="P69" s="5"/>
+      <c r="C67" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="68" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="70" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>9</v>
+        <v>125</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="71" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="4"/>
-      <c r="G74" s="4"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="4"/>
-      <c r="J74" s="4"/>
-      <c r="K74" s="4"/>
-      <c r="L74" s="5"/>
-      <c r="M74" s="4"/>
-      <c r="N74" s="4"/>
-      <c r="O74" s="4"/>
-      <c r="P74" s="5"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="73" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="75" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>9</v>
+        <v>135</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="76" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
-      <c r="G79" s="4"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="4"/>
-      <c r="J79" s="4"/>
-      <c r="K79" s="4"/>
-      <c r="L79" s="5"/>
-      <c r="M79" s="4"/>
-      <c r="N79" s="4"/>
-      <c r="O79" s="4"/>
-      <c r="P79" s="5"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="76" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="78" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="79" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="80" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>9</v>
+        <v>142</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="81" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="81" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
     <row r="82" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>129</v>
+        <v>146</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="83" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>132</v>
+        <v>148</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="84" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="85" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
-      <c r="H88" s="5"/>
-      <c r="I88" s="4"/>
-      <c r="J88" s="4"/>
-      <c r="K88" s="4"/>
-      <c r="L88" s="5"/>
-      <c r="M88" s="4"/>
-      <c r="N88" s="4"/>
-      <c r="O88" s="4"/>
-      <c r="P88" s="5"/>
+        <v>150</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="85" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="86" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="87" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="88" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="89" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>7</v>
+        <v>160</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="90" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="91" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="90" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="91" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
     <row r="93" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
     </row>
     <row r="94" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>170</v>
+      </c>
       <c r="C94" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="95" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="95" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
     <row r="96" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>141</v>
+        <v>174</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>142</v>
+        <v>175</v>
       </c>
     </row>
     <row r="97" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>176</v>
+      </c>
       <c r="C97" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="98" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="98" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
     <row r="99" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="100" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="C100" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="101" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="C101" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="102" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="C102" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="103" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="C103" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="1" t="s">
-        <v>150</v>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="104" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="105" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="106" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>193</v>
+      </c>
       <c r="C106" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="107" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="C107" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C108" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="C109" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
+        <v>200</v>
+      </c>
       <c r="C110" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="C111" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="C114" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C115" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="C116" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C117" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="s">
+        <v>215</v>
+      </c>
       <c r="C118" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="1" t="s">
-        <v>164</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="119" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C121" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B123" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C124" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B126" s="1" t="s">
-        <v>169</v>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4"/>
+      <c r="H125" s="5"/>
+      <c r="I125" s="4"/>
+      <c r="J125" s="4"/>
+      <c r="K125" s="4"/>
+      <c r="L125" s="5"/>
+      <c r="M125" s="4"/>
+      <c r="N125" s="4"/>
+      <c r="O125" s="4"/>
+      <c r="P125" s="5"/>
+    </row>
+    <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C127" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
+        <v>228</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C130" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B130" s="4"/>
+      <c r="C130" s="4"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="4"/>
+      <c r="F130" s="4"/>
+      <c r="G130" s="4"/>
+      <c r="H130" s="5"/>
+      <c r="I130" s="4"/>
+      <c r="J130" s="4"/>
+      <c r="K130" s="4"/>
+      <c r="L130" s="5"/>
+      <c r="M130" s="4"/>
+      <c r="N130" s="4"/>
+      <c r="O130" s="4"/>
+      <c r="P130" s="5"/>
+    </row>
+    <row r="131" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C131" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C132" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C133" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C134" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="133" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C135" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C138" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B135" s="4"/>
+      <c r="C135" s="4"/>
+      <c r="D135" s="5"/>
+      <c r="E135" s="4"/>
+      <c r="F135" s="4"/>
+      <c r="G135" s="4"/>
+      <c r="H135" s="5"/>
+      <c r="I135" s="4"/>
+      <c r="J135" s="4"/>
+      <c r="K135" s="4"/>
+      <c r="L135" s="5"/>
+      <c r="M135" s="4"/>
+      <c r="N135" s="4"/>
+      <c r="O135" s="4"/>
+      <c r="P135" s="5"/>
+    </row>
+    <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C141" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C142" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C143" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>240</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B144" s="4"/>
+      <c r="C144" s="4"/>
+      <c r="D144" s="5"/>
+      <c r="E144" s="4"/>
+      <c r="F144" s="4"/>
+      <c r="G144" s="4"/>
+      <c r="H144" s="5"/>
+      <c r="I144" s="4"/>
+      <c r="J144" s="4"/>
+      <c r="K144" s="4"/>
+      <c r="L144" s="5"/>
+      <c r="M144" s="4"/>
+      <c r="N144" s="4"/>
+      <c r="O144" s="4"/>
+      <c r="P144" s="5"/>
+    </row>
+    <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>186</v>
+        <v>7</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0"/>
-      <c r="C146" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C147" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C148" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="1" t="s">
-        <v>190</v>
-      </c>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C150" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C151" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="s">
+        <v>248</v>
+      </c>
       <c r="C152" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C153" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
-        <v>194</v>
+        <v>251</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>195</v>
+        <v>253</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C156" s="1" t="s">
-        <v>196</v>
+        <v>254</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C157" s="1" t="s">
-        <v>197</v>
+        <v>255</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C158" s="1" t="s">
-        <v>198</v>
+        <v>256</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C159" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C160" s="1" t="s">
-        <v>200</v>
+        <v>247</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B161" s="1" t="s">
+        <v>257</v>
+      </c>
       <c r="C161" s="1" t="s">
-        <v>201</v>
+        <v>258</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C162" s="1" t="s">
-        <v>202</v>
+        <v>259</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C163" s="1" t="s">
-        <v>189</v>
+        <v>260</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="0"/>
+      <c r="C164" s="1" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="C165" s="1" t="s">
-        <v>187</v>
+        <v>262</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C166" s="1" t="s">
-        <v>204</v>
+        <v>263</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C167" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C168" s="1" t="s">
-        <v>206</v>
+        <v>264</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B169" s="1" t="s">
+        <v>265</v>
+      </c>
       <c r="C169" s="1" t="s">
-        <v>188</v>
+        <v>266</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C170" s="1" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C171" s="1" t="s">
-        <v>189</v>
+        <v>268</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B172" s="0"/>
+      <c r="C172" s="1" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B173" s="1" t="s">
-        <v>208</v>
-      </c>
       <c r="C173" s="1" t="s">
-        <v>209</v>
+        <v>270</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C174" s="1" t="s">
-        <v>166</v>
+        <v>264</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B176" s="1" t="s">
-        <v>210</v>
+        <v>271</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>211</v>
+        <v>272</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C177" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C178" s="1" t="s">
-        <v>166</v>
+        <v>273</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="0"/>
+      <c r="B179" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="1" t="s">
-        <v>213</v>
-      </c>
       <c r="C180" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C181" s="1" t="s">
-        <v>189</v>
+        <v>273</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B182" s="0"/>
+      <c r="B182" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B183" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="C183" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C184" s="1" t="s">
-        <v>188</v>
+        <v>273</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="1" t="s">
+        <v>278</v>
+      </c>
       <c r="C185" s="1" t="s">
-        <v>217</v>
+        <v>279</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C186" s="1" t="s">
-        <v>189</v>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C187" s="1" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="C188" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="G188" s="7"/>
+        <v>282</v>
+      </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C189" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="G189" s="7"/>
+        <v>283</v>
+      </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C190" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="G190" s="7"/>
+        <v>284</v>
+      </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C191" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="G191" s="7"/>
-    </row>
-    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C192" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G192" s="7"/>
+        <v>285</v>
+      </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>287</v>
+      </c>
       <c r="C193" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="G193" s="7"/>
+        <v>288</v>
+      </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C194" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G194" s="7"/>
-    </row>
-    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C195" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="G195" s="7"/>
+        <v>247</v>
+      </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="1" t="s">
+        <v>289</v>
+      </c>
       <c r="C196" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="G196" s="7"/>
+        <v>290</v>
+      </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C197" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="G197" s="7"/>
+        <v>291</v>
+      </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B198" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="C198" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G198" s="7"/>
+        <v>292</v>
+      </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G199" s="7"/>
-    </row>
-    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C200" s="1" t="s">
-        <v>230</v>
+      <c r="C199" s="1" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="C201" s="1" t="s">
-        <v>231</v>
+        <v>294</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0"/>
       <c r="C202" s="1" t="s">
-        <v>232</v>
+        <v>279</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C203" s="1" t="s">
-        <v>233</v>
+        <v>295</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C204" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C205" s="1" t="s">
-        <v>235</v>
+        <v>296</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="1" t="s">
+        <v>297</v>
+      </c>
       <c r="C206" s="1" t="s">
-        <v>236</v>
+        <v>298</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C207" s="1" t="s">
-        <v>237</v>
+        <v>299</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C208" s="1" t="s">
-        <v>217</v>
+        <v>300</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C209" s="1" t="s">
-        <v>189</v>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C212" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C213" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C214" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C215" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C216" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C217" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C218" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C219" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0"/>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C222" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C223" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C224" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C225" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C226" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C227" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B228" s="0"/>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B229" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C230" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B232" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C233" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C234" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0"/>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C237" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B238" s="0"/>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B239" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C240" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C241" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C242" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C245" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C246" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C247" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C248" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C249" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C250" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C251" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C252" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C253" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B254" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C257" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C258" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C259" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C260" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C261" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C262" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C263" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C264" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C265" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C269" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C272" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B275" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C276" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C277" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C278" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C279" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C280" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B282" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C283" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C284" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C285" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C286" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C287" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C288" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B290" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C291" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C292" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C293" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C294" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C295" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C296" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C297" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B299" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C300" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C301" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B303" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B305" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C306" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C307" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C308" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C309" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C310" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C311" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C312" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C313" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C314" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B316" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C317" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C318" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C319" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C320" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C321" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B323" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C324" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B326" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C327" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B329" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C330" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B332" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C333" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B335" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C336" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B338" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C339" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C340" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C341" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B343" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C344" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B346" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C347" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B349" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C350" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C351" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C352" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C353" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C354" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C355" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C356" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B358" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C359" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B361" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C361" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C362" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C363" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C364" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C365" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C366" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C367" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C368" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B370" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C371" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B373" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C374" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B376" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C377" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B379" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C380" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B382" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C382" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C383" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B385" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C385" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C386" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C387" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B389" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C389" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C390" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C391" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C392" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B394" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C394" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C395" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C396" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C397" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C398" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C399" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C400" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B402" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C402" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C403" s="1" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C404" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C405" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C406" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C407" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C408" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C409" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B411" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C411" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C412" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C413" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C414" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B416" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C416" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C417" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B419" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C419" s="1" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C420" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B422" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C422" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C423" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B425" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C425" s="1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C426" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B428" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C428" s="1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C429" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B431" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C431" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C432" s="1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C433" s="1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C434" s="1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C435" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C436" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C437" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B439" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="C439" s="1" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C440" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C441" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C442" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C443" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C444" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C445" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C446" s="1" t="s">
+        <v>482</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C115" r:id="rId1" display="https://vk.com/@svitolina-elina-svitolina-s-kontoi-nam-predstoit-esche-odna-bitva"/>
+    <hyperlink ref="C117" r:id="rId2" display="http://svitolina.com/ru/news/456-news-04-01.html"/>
+    <hyperlink ref="C119" r:id="rId3" display="https://vk.com/@svitolina-elina-svitolina-taibreik-vo-vtorom-sete-ya-otygrala-na-vse-1"/>
+    <hyperlink ref="C121" r:id="rId4" display="https://vk.com/@svitolina-elina-svitolina-otkryvat-sezon-pobedoi-na-turnire-eto-vseg"/>
+    <hyperlink ref="C123" r:id="rId5" display="https://vk.com/@svitolina-elina-svitolina-nadeus-ya-horoshaya-aktrisa-i-vy-ne-zametili"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
howdoi / execute howdoi
</commit_message>
<xml_diff>
--- a/_bots/gorkathebot/gorkathebot.xlsx
+++ b/_bots/gorkathebot/gorkathebot.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">VERSION</t>
   </si>
   <si>
-    <t xml:space="preserve">0.4.0</t>
+    <t xml:space="preserve">0.4.1</t>
   </si>
   <si>
     <t xml:space="preserve">gorkathebot</t>
@@ -913,7 +913,7 @@
     <t xml:space="preserve">IF EQ botMode optInitialBot THEN GOTO oldstart</t>
   </si>
   <si>
-    <t xml:space="preserve">IF EQ botMode optHowdoi THEN GOTO howdoi</t>
+    <t xml:space="preserve">IF EQ botMode optHowdoiBot THEN GOTO howdoi</t>
   </si>
   <si>
     <t xml:space="preserve">END</t>
@@ -2053,8 +2053,8 @@
   </sheetPr>
   <dimension ref="A1:P539"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A150" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B176" activeCellId="0" sqref="B176"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fix render of multiline preformatted text (2)
</commit_message>
<xml_diff>
--- a/_bots/gorkathebot/gorkathebot.xlsx
+++ b/_bots/gorkathebot/gorkathebot.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="592">
   <si>
     <t xml:space="preserve">BOTBASIC</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">VERSION</t>
   </si>
   <si>
-    <t xml:space="preserve">0.4.1</t>
+    <t xml:space="preserve">0.4.3</t>
   </si>
   <si>
     <t xml:space="preserve">gorkathebot</t>
@@ -790,10 +790,22 @@
     <t xml:space="preserve">{a}</t>
   </si>
   <si>
+    <t xml:space="preserve">lnk_hdi_wikipedia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://en.wikipedia.org/w/index.php?search={q}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lnk_hdi_google</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.google.com/search?hl=en&amp;q={q}</t>
+  </si>
+  <si>
     <t xml:space="preserve">txt_hdi_wikipedia</t>
   </si>
   <si>
-    <t xml:space="preserve">Take a look at https://en.wikipedia.org/w/index.php?search={q}</t>
+    <t xml:space="preserve">Take a look at {lnk_hdi_wikipedia} and {lnk_hdi_google}</t>
   </si>
   <si>
     <t xml:space="preserve">rem_hdi_section_end</t>
@@ -2051,7 +2063,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P539"/>
+  <dimension ref="A1:P541"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
@@ -3163,1951 +3175,1967 @@
       <c r="A148" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="C148" s="1" t="s">
+      <c r="C148" s="8" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="1" t="s">
-        <v>258</v>
+      <c r="A150" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B154" s="4"/>
-      <c r="C154" s="4"/>
-      <c r="D154" s="5"/>
-      <c r="E154" s="4"/>
-      <c r="F154" s="4"/>
-      <c r="G154" s="4"/>
-      <c r="H154" s="5"/>
-      <c r="I154" s="4"/>
-      <c r="J154" s="4"/>
-      <c r="K154" s="4"/>
-      <c r="L154" s="5"/>
-      <c r="M154" s="4"/>
-      <c r="N154" s="4"/>
-      <c r="O154" s="4"/>
-      <c r="P154" s="5"/>
-    </row>
-    <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="1" t="s">
+    <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B156" s="4"/>
+      <c r="C156" s="4"/>
+      <c r="D156" s="5"/>
+      <c r="E156" s="4"/>
+      <c r="F156" s="4"/>
+      <c r="G156" s="4"/>
+      <c r="H156" s="5"/>
+      <c r="I156" s="4"/>
+      <c r="J156" s="4"/>
+      <c r="K156" s="4"/>
+      <c r="L156" s="5"/>
+      <c r="M156" s="4"/>
+      <c r="N156" s="4"/>
+      <c r="O156" s="4"/>
+      <c r="P156" s="5"/>
+    </row>
+    <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C155" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="F155" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="G155" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C157" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
     <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="3" t="s">
+    <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B161" s="4"/>
+      <c r="C161" s="4"/>
+      <c r="D161" s="5"/>
+      <c r="E161" s="4"/>
+      <c r="F161" s="4"/>
+      <c r="G161" s="4"/>
+      <c r="H161" s="5"/>
+      <c r="I161" s="4"/>
+      <c r="J161" s="4"/>
+      <c r="K161" s="4"/>
+      <c r="L161" s="5"/>
+      <c r="M161" s="4"/>
+      <c r="N161" s="4"/>
+      <c r="O161" s="4"/>
+      <c r="P161" s="5"/>
+    </row>
+    <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C162" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B159" s="4"/>
-      <c r="C159" s="4"/>
-      <c r="D159" s="5"/>
-      <c r="E159" s="4"/>
-      <c r="F159" s="4"/>
-      <c r="G159" s="4"/>
-      <c r="H159" s="5"/>
-      <c r="I159" s="4"/>
-      <c r="J159" s="4"/>
-      <c r="K159" s="4"/>
-      <c r="L159" s="5"/>
-      <c r="M159" s="4"/>
-      <c r="N159" s="4"/>
-      <c r="O159" s="4"/>
-      <c r="P159" s="5"/>
-    </row>
-    <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
     <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="B164" s="4"/>
-      <c r="C164" s="4"/>
-      <c r="D164" s="5"/>
-      <c r="E164" s="4"/>
-      <c r="F164" s="4"/>
-      <c r="G164" s="4"/>
-      <c r="H164" s="5"/>
-      <c r="I164" s="4"/>
-      <c r="J164" s="4"/>
-      <c r="K164" s="4"/>
-      <c r="L164" s="5"/>
-      <c r="M164" s="4"/>
-      <c r="N164" s="4"/>
-      <c r="O164" s="4"/>
-      <c r="P164" s="5"/>
-    </row>
-    <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="F165" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="G165" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B166" s="4"/>
+      <c r="C166" s="4"/>
+      <c r="D166" s="5"/>
+      <c r="E166" s="4"/>
+      <c r="F166" s="4"/>
+      <c r="G166" s="4"/>
+      <c r="H166" s="5"/>
+      <c r="I166" s="4"/>
+      <c r="J166" s="4"/>
+      <c r="K166" s="4"/>
+      <c r="L166" s="5"/>
+      <c r="M166" s="4"/>
+      <c r="N166" s="4"/>
+      <c r="O166" s="4"/>
+      <c r="P166" s="5"/>
+    </row>
     <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F167" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="E167" s="1" t="s">
+      <c r="G167" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="F167" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F168" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
+    </row>
+    <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F169" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F169" s="1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F170" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F170" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="G170" s="1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G172" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F172" s="1" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="F173" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F173" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E174" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>283</v>
       </c>
       <c r="F174" s="1" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
     <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="B180" s="4"/>
-      <c r="C180" s="4"/>
-      <c r="D180" s="5"/>
-      <c r="E180" s="4"/>
-      <c r="F180" s="4"/>
-      <c r="G180" s="4"/>
-      <c r="H180" s="5"/>
-      <c r="I180" s="4"/>
-      <c r="J180" s="4"/>
-      <c r="K180" s="4"/>
-      <c r="L180" s="5"/>
-      <c r="M180" s="4"/>
-      <c r="N180" s="4"/>
-      <c r="O180" s="4"/>
-      <c r="P180" s="5"/>
-    </row>
-    <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="1" t="s">
+    <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B182" s="4"/>
+      <c r="C182" s="4"/>
+      <c r="D182" s="5"/>
+      <c r="E182" s="4"/>
+      <c r="F182" s="4"/>
+      <c r="G182" s="4"/>
+      <c r="H182" s="5"/>
+      <c r="I182" s="4"/>
+      <c r="J182" s="4"/>
+      <c r="K182" s="4"/>
+      <c r="L182" s="5"/>
+      <c r="M182" s="4"/>
+      <c r="N182" s="4"/>
+      <c r="O182" s="4"/>
+      <c r="P182" s="5"/>
+    </row>
+    <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B181" s="1" t="s">
+      <c r="B183" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C181" s="1" t="s">
+      <c r="C183" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="C185" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C186" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
+    <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>298</v>
+      </c>
       <c r="C187" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C188" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C189" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="B190" s="1" t="s">
-        <v>300</v>
-      </c>
       <c r="C190" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C191" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="1" t="s">
+      <c r="C193" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="C193" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C194" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
     <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>306</v>
-      </c>
       <c r="C196" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C197" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="C198" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C199" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C200" s="1" t="s">
-        <v>298</v>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C201" s="1" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B202" s="1" t="s">
-        <v>311</v>
-      </c>
       <c r="C202" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C203" s="1" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B204" s="1" t="s">
+        <v>315</v>
+      </c>
       <c r="C204" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C205" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C206" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C207" s="1" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C208" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C209" s="1" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B210" s="1" t="s">
-        <v>319</v>
-      </c>
       <c r="C210" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C211" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B212" s="1" t="s">
+        <v>323</v>
+      </c>
       <c r="C212" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C213" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C214" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C215" s="1" t="s">
-        <v>318</v>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C216" s="1" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B217" s="1" t="s">
-        <v>325</v>
-      </c>
       <c r="C217" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C218" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B219" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B220" s="1" t="s">
-        <v>328</v>
-      </c>
       <c r="C220" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C221" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B222" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B223" s="1" t="s">
-        <v>330</v>
-      </c>
       <c r="C223" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C224" s="1" t="s">
-        <v>327</v>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B225" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="1" t="s">
-        <v>332</v>
-      </c>
       <c r="C226" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C227" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="1" t="s">
+        <v>336</v>
+      </c>
       <c r="C228" s="1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C229" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C230" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C231" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C232" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C233" s="1" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="B234" s="1" t="s">
-        <v>341</v>
-      </c>
       <c r="C234" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C235" s="1" t="s">
-        <v>298</v>
+        <v>343</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="1" t="s">
-        <v>343</v>
-      </c>
       <c r="C237" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C238" s="1" t="s">
-        <v>345</v>
+        <v>302</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="1" t="s">
+        <v>347</v>
+      </c>
       <c r="C239" s="1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C240" s="1" t="s">
-        <v>298</v>
+        <v>349</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C241" s="1" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="1" t="s">
-        <v>347</v>
-      </c>
       <c r="C242" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="0"/>
-      <c r="C243" s="1" t="s">
-        <v>333</v>
+        <v>302</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="1" t="s">
+        <v>351</v>
+      </c>
       <c r="C244" s="1" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="0"/>
       <c r="C245" s="1" t="s">
-        <v>350</v>
+        <v>337</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C246" s="1" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="1" t="s">
-        <v>351</v>
-      </c>
       <c r="C247" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C248" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="1" t="s">
+        <v>355</v>
+      </c>
       <c r="C249" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C250" s="1" t="s">
-        <v>350</v>
+        <v>357</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C251" s="1" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="1" t="s">
-        <v>355</v>
-      </c>
       <c r="C252" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C253" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="1" t="s">
+        <v>359</v>
+      </c>
       <c r="C254" s="1" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C255" s="1" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C256" s="1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C257" s="1" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C258" s="1" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C259" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C260" s="1" t="s">
-        <v>350</v>
+        <v>366</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="0"/>
+      <c r="C261" s="1" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="1" t="s">
-        <v>364</v>
-      </c>
       <c r="C262" s="1" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C263" s="1" t="s">
-        <v>365</v>
-      </c>
+      <c r="A263" s="0"/>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="1" t="s">
+        <v>368</v>
+      </c>
       <c r="C264" s="1" t="s">
-        <v>366</v>
+        <v>352</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C265" s="1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C266" s="1" t="s">
-        <v>349</v>
+        <v>370</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C267" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C268" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B269" s="0"/>
+      <c r="C269" s="1" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B270" s="1" t="s">
-        <v>369</v>
-      </c>
       <c r="C270" s="1" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C271" s="1" t="s">
-        <v>327</v>
+      <c r="B271" s="0"/>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B272" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B273" s="1" t="s">
-        <v>371</v>
-      </c>
       <c r="C273" s="1" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C274" s="1" t="s">
-        <v>373</v>
+        <v>331</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B275" s="1" t="s">
+        <v>375</v>
+      </c>
       <c r="C275" s="1" t="s">
-        <v>327</v>
+        <v>376</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="0"/>
+      <c r="C276" s="1" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="1" t="s">
-        <v>374</v>
-      </c>
       <c r="C277" s="1" t="s">
-        <v>375</v>
+        <v>331</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C278" s="1" t="s">
-        <v>350</v>
-      </c>
+      <c r="A278" s="0"/>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B279" s="0"/>
+      <c r="A279" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B280" s="1" t="s">
-        <v>376</v>
-      </c>
       <c r="C280" s="1" t="s">
-        <v>377</v>
+        <v>354</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C281" s="1" t="s">
-        <v>349</v>
-      </c>
+      <c r="B281" s="0"/>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B282" s="1" t="s">
+        <v>380</v>
+      </c>
       <c r="C282" s="1" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C283" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C284" s="1" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="1" t="s">
-        <v>379</v>
-      </c>
       <c r="C285" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C286" s="1" t="s">
-        <v>381</v>
+        <v>354</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="1" t="s">
+        <v>383</v>
+      </c>
       <c r="C287" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C288" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C289" s="1" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C290" s="1" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C291" s="1" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C292" s="1" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C293" s="1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C294" s="1" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B295" s="1" t="s">
-        <v>389</v>
-      </c>
       <c r="C295" s="1" t="s">
-        <v>350</v>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C296" s="1" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="1" t="s">
-        <v>390</v>
+      <c r="B297" s="1" t="s">
+        <v>393</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C298" s="1" t="s">
-        <v>392</v>
+        <v>354</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="1" t="s">
+        <v>394</v>
+      </c>
       <c r="C299" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C300" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C301" s="1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C302" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C303" s="1" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C304" s="1" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C305" s="1" t="s">
-        <v>378</v>
+        <v>401</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C306" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C310" s="1" t="s">
-        <v>399</v>
+        <v>402</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C307" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C308" s="1" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="1" t="s">
-        <v>400</v>
-      </c>
       <c r="C312" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C313" s="1" t="s">
-        <v>298</v>
+        <v>403</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="B315" s="1" t="s">
-        <v>403</v>
-      </c>
       <c r="C315" s="1" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B316" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="C316" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="1" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B317" s="1" t="s">
+        <v>407</v>
+      </c>
       <c r="C317" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B318" s="1" t="s">
+        <v>409</v>
+      </c>
       <c r="C318" s="1" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C319" s="1" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C320" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C321" s="1" t="s">
-        <v>339</v>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C322" s="1" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B323" s="1" t="s">
-        <v>411</v>
-      </c>
       <c r="C323" s="1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C324" s="1" t="s">
-        <v>413</v>
+        <v>343</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B325" s="1" t="s">
+        <v>415</v>
+      </c>
       <c r="C325" s="1" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C326" s="1" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C327" s="1" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C328" s="1" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C329" s="1" t="s">
-        <v>327</v>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C330" s="1" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B331" s="1" t="s">
-        <v>418</v>
-      </c>
       <c r="C331" s="1" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C332" s="1" t="s">
-        <v>420</v>
+        <v>331</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B333" s="1" t="s">
+        <v>422</v>
+      </c>
       <c r="C333" s="1" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C334" s="1" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C335" s="1" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C336" s="1" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C337" s="1" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C338" s="1" t="s">
-        <v>327</v>
+        <v>428</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C339" s="1" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B340" s="1" t="s">
-        <v>426</v>
-      </c>
       <c r="C340" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C341" s="1" t="s">
-        <v>428</v>
+        <v>331</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B342" s="1" t="s">
+        <v>430</v>
+      </c>
       <c r="C342" s="1" t="s">
-        <v>327</v>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C343" s="1" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B344" s="1" t="s">
-        <v>429</v>
-      </c>
       <c r="C344" s="1" t="s">
-        <v>430</v>
+        <v>331</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B346" s="1" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C347" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B348" s="1" t="s">
+        <v>435</v>
+      </c>
       <c r="C348" s="1" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C349" s="1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C350" s="1" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C351" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C352" s="1" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C353" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C354" s="1" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C355" s="1" t="s">
-        <v>327</v>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C356" s="1" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B357" s="1" t="s">
-        <v>441</v>
-      </c>
       <c r="C357" s="1" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C358" s="1" t="s">
-        <v>443</v>
+        <v>331</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B359" s="1" t="s">
+        <v>445</v>
+      </c>
       <c r="C359" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C360" s="1" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C361" s="1" t="s">
-        <v>378</v>
+        <v>448</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C362" s="1" t="s">
-        <v>327</v>
+        <v>449</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C363" s="1" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B364" s="1" t="s">
-        <v>446</v>
-      </c>
       <c r="C364" s="1" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C365" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B366" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C366" s="1" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B367" s="1" t="s">
-        <v>448</v>
-      </c>
       <c r="C367" s="1" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C368" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B369" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C369" s="1" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B370" s="1" t="s">
-        <v>450</v>
-      </c>
       <c r="C370" s="1" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C371" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B372" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B373" s="1" t="s">
-        <v>452</v>
-      </c>
       <c r="C373" s="1" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C374" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B375" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="C375" s="1" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B376" s="1" t="s">
-        <v>454</v>
-      </c>
       <c r="C376" s="1" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C377" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B378" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B379" s="1" t="s">
-        <v>456</v>
-      </c>
       <c r="C379" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C380" s="1" t="s">
-        <v>458</v>
+        <v>331</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B381" s="1" t="s">
+        <v>460</v>
+      </c>
       <c r="C381" s="1" t="s">
-        <v>425</v>
+        <v>461</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C382" s="1" t="s">
-        <v>327</v>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C383" s="1" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B384" s="1" t="s">
-        <v>459</v>
-      </c>
       <c r="C384" s="1" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C385" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B386" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C386" s="1" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B387" s="1" t="s">
-        <v>461</v>
-      </c>
       <c r="C387" s="1" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C388" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B389" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C389" s="1" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B390" s="1" t="s">
-        <v>463</v>
-      </c>
       <c r="C390" s="1" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C391" s="1" t="s">
-        <v>465</v>
+        <v>331</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B392" s="1" t="s">
+        <v>467</v>
+      </c>
       <c r="C392" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C393" s="1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C394" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C395" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C396" s="1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C397" s="1" t="s">
-        <v>327</v>
+        <v>473</v>
+      </c>
+    </row>
+    <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C398" s="1" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B399" s="1" t="s">
-        <v>471</v>
-      </c>
       <c r="C399" s="1" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C400" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B401" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C401" s="1" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B402" s="1" t="s">
-        <v>473</v>
-      </c>
       <c r="C402" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C403" s="1" t="s">
-        <v>474</v>
+        <v>331</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B404" s="1" t="s">
+        <v>477</v>
+      </c>
       <c r="C404" s="1" t="s">
-        <v>475</v>
+        <v>436</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C405" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C406" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C407" s="1" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C408" s="1" t="s">
-        <v>417</v>
+        <v>481</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C409" s="1" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C410" s="1" t="s">
-        <v>480</v>
+        <v>421</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C411" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C412" s="1" t="s">
-        <v>327</v>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C413" s="1" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B414" s="1" t="s">
-        <v>482</v>
-      </c>
       <c r="C414" s="1" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C415" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B416" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C416" s="1" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B417" s="1" t="s">
-        <v>484</v>
-      </c>
       <c r="C417" s="1" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C418" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B419" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C419" s="1" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B420" s="1" t="s">
-        <v>486</v>
-      </c>
       <c r="C420" s="1" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C421" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B422" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C422" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B423" s="1" t="s">
-        <v>488</v>
-      </c>
       <c r="C423" s="1" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C424" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B425" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C425" s="1" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B426" s="1" t="s">
-        <v>490</v>
-      </c>
       <c r="C426" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C427" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B428" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C428" s="1" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B429" s="1" t="s">
-        <v>492</v>
-      </c>
       <c r="C429" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C430" s="1" t="s">
-        <v>493</v>
+        <v>331</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B431" s="1" t="s">
+        <v>496</v>
+      </c>
       <c r="C431" s="1" t="s">
-        <v>327</v>
+        <v>436</v>
+      </c>
+    </row>
+    <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C432" s="1" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B433" s="1" t="s">
-        <v>494</v>
-      </c>
       <c r="C433" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C434" s="1" t="s">
-        <v>495</v>
+        <v>331</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B435" s="1" t="s">
+        <v>498</v>
+      </c>
       <c r="C435" s="1" t="s">
-        <v>493</v>
+        <v>436</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C436" s="1" t="s">
-        <v>327</v>
+        <v>499</v>
+      </c>
+    </row>
+    <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C437" s="1" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B438" s="1" t="s">
-        <v>496</v>
-      </c>
       <c r="C438" s="1" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C439" s="1" t="s">
-        <v>498</v>
+        <v>331</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B440" s="1" t="s">
+        <v>500</v>
+      </c>
       <c r="C440" s="1" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C441" s="1" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C442" s="1" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C443" s="1" t="s">
-        <v>425</v>
+        <v>504</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C444" s="1" t="s">
-        <v>327</v>
+        <v>505</v>
+      </c>
+    </row>
+    <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C445" s="1" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B446" s="1" t="s">
-        <v>502</v>
-      </c>
       <c r="C446" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C447" s="1" t="s">
-        <v>503</v>
+        <v>331</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B448" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="C448" s="1" t="s">
-        <v>504</v>
+        <v>436</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C449" s="1" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C450" s="1" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C451" s="1" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C452" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C453" s="1" t="s">
-        <v>327</v>
+        <v>511</v>
+      </c>
+    </row>
+    <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C454" s="1" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B455" s="1" t="s">
-        <v>509</v>
-      </c>
       <c r="C455" s="1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C456" s="1" t="s">
-        <v>511</v>
+        <v>331</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B457" s="1" t="s">
+        <v>513</v>
+      </c>
       <c r="C457" s="1" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C458" s="1" t="s">
-        <v>327</v>
+        <v>515</v>
+      </c>
+    </row>
+    <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C459" s="1" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B460" s="1" t="s">
-        <v>513</v>
-      </c>
       <c r="C460" s="1" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C461" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B462" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="C462" s="1" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B463" s="1" t="s">
-        <v>515</v>
-      </c>
       <c r="C463" s="1" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C464" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B465" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C465" s="1" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B466" s="1" t="s">
-        <v>517</v>
-      </c>
       <c r="C466" s="1" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C467" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B468" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C468" s="1" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B469" s="1" t="s">
-        <v>519</v>
-      </c>
       <c r="C469" s="1" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C470" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B471" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="C471" s="1" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B472" s="1" t="s">
-        <v>521</v>
-      </c>
       <c r="C472" s="1" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C473" s="1" t="s">
-        <v>327</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B474" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C474" s="1" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B475" s="1" t="s">
-        <v>523</v>
-      </c>
       <c r="C475" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C476" s="1" t="s">
-        <v>524</v>
+        <v>331</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B477" s="1" t="s">
+        <v>527</v>
+      </c>
       <c r="C477" s="1" t="s">
-        <v>525</v>
+        <v>436</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C478" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C479" s="1" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C480" s="1" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C481" s="1" t="s">
-        <v>529</v>
+        <v>531</v>
+      </c>
+    </row>
+    <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C482" s="1" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B483" s="1" t="s">
-        <v>530</v>
-      </c>
       <c r="C483" s="1" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C484" s="1" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B485" s="1" t="s">
+        <v>534</v>
+      </c>
       <c r="C485" s="1" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C486" s="1" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C487" s="1" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C488" s="1" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C489" s="1" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C490" s="1" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A494" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="B494" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="C494" s="1" t="s">
+    </row>
+    <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C491" s="1" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C495" s="1" t="s">
+    <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C492" s="1" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A496" s="1" t="s">
+        <v>543</v>
+      </c>
       <c r="B496" s="1" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C496" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C497" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B498" s="1" t="s">
+        <v>547</v>
+      </c>
       <c r="C498" s="1" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C499" s="1" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C500" s="1" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C501" s="1" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C502" s="1" t="s">
-        <v>550</v>
+        <v>552</v>
+      </c>
+    </row>
+    <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C503" s="1" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A504" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="B504" s="1" t="s">
-        <v>552</v>
-      </c>
       <c r="C504" s="1" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B505" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="C505" s="1" t="s">
+    </row>
+    <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A506" s="1" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B506" s="1" t="s">
+        <v>556</v>
+      </c>
       <c r="C506" s="1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B507" s="1" t="s">
+        <v>558</v>
+      </c>
       <c r="C507" s="1" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C508" s="1" t="s">
-        <v>327</v>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C509" s="1" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B510" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="C510" s="1" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C511" s="1" t="s">
-        <v>560</v>
+        <v>331</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B512" s="1" t="s">
+        <v>562</v>
+      </c>
       <c r="C512" s="1" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C513" s="1" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C514" s="1" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C515" s="1" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C516" s="1" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B517" s="1" t="s">
-        <v>566</v>
-      </c>
       <c r="C517" s="1" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B518" s="1" t="s">
-        <v>568</v>
-      </c>
       <c r="C518" s="1" t="s">
         <v>569</v>
       </c>
     </row>
+    <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B519" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="C519" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
     <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B520" s="1" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="C520" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C521" s="1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B522" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="C522" s="1" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C523" s="8" t="s">
-        <v>574</v>
+      <c r="C523" s="1" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C524" s="8" t="s">
-        <v>575</v>
+      <c r="C524" s="1" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C525" s="8" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B526" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="C526" s="1" t="s">
-        <v>578</v>
+      <c r="C526" s="8" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C527" s="8" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B528" s="1" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="C528" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C529" s="1" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B530" s="1" t="s">
+        <v>583</v>
+      </c>
       <c r="C530" s="1" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C531" s="1" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C532" s="1" t="s">
-        <v>576</v>
+        <v>585</v>
+      </c>
+    </row>
+    <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C533" s="1" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B534" s="1" t="s">
-        <v>583</v>
-      </c>
       <c r="C534" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C535" s="1" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B536" s="1" t="s">
+        <v>587</v>
+      </c>
       <c r="C536" s="1" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C537" s="1" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C538" s="1" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C539" s="1" t="s">
-        <v>327</v>
+        <v>590</v>
+      </c>
+    </row>
+    <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C540" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C541" s="1" t="s">
+        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix process of templates with subtemplates
</commit_message>
<xml_diff>
--- a/_bots/gorkathebot/gorkathebot.xlsx
+++ b/_bots/gorkathebot/gorkathebot.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">VERSION</t>
   </si>
   <si>
-    <t xml:space="preserve">0.4.3</t>
+    <t xml:space="preserve">0.4.4</t>
   </si>
   <si>
     <t xml:space="preserve">gorkathebot</t>
@@ -802,10 +802,43 @@
     <t xml:space="preserve">https://www.google.com/search?hl=en&amp;q={q}</t>
   </si>
   <si>
-    <t xml:space="preserve">txt_hdi_wikipedia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Take a look at {lnk_hdi_wikipedia} and {lnk_hdi_google}</t>
+    <t xml:space="preserve">txt_hdi_links</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Take a look at </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{lnk_hdi_google}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{lnk_hdi_wikipedia}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">rem_hdi_section_end</t>
@@ -1843,7 +1876,23 @@
     <t xml:space="preserve">CALL UrlEncode q TO q</t>
   </si>
   <si>
-    <t xml:space="preserve">PRINT txt_hdi_wikipedia</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PRINT </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">txt_hdi_links</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2066,7 +2115,7 @@
   <dimension ref="A1:P541"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fix render of http links with display text
</commit_message>
<xml_diff>
--- a/_bots/gorkathebot/gorkathebot.xlsx
+++ b/_bots/gorkathebot/gorkathebot.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">VERSION</t>
   </si>
   <si>
-    <t xml:space="preserve">0.4.4</t>
+    <t xml:space="preserve">0.4.5</t>
   </si>
   <si>
     <t xml:space="preserve">gorkathebot</t>
@@ -793,13 +793,13 @@
     <t xml:space="preserve">lnk_hdi_wikipedia</t>
   </si>
   <si>
-    <t xml:space="preserve">https://en.wikipedia.org/w/index.php?search={q}</t>
+    <t xml:space="preserve">https:Wikipedia://en.wikipedia.org/w/index.php?search={q}</t>
   </si>
   <si>
     <t xml:space="preserve">lnk_hdi_google</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.google.com/search?hl=en&amp;q={q}</t>
+    <t xml:space="preserve">https:Google://www.google.com/search?hl=en&amp;q={q}</t>
   </si>
   <si>
     <t xml:space="preserve">txt_hdi_links</t>
@@ -2114,8 +2114,8 @@
   </sheetPr>
   <dimension ref="A1:P541"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A136" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C149" activeCellId="0" sqref="C149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
enable render of http links inside preformatted text
</commit_message>
<xml_diff>
--- a/_bots/gorkathebot/gorkathebot.xlsx
+++ b/_bots/gorkathebot/gorkathebot.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="605">
   <si>
     <t xml:space="preserve">BOTBASIC</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">VERSION</t>
   </si>
   <si>
-    <t xml:space="preserve">0.4.5</t>
+    <t xml:space="preserve">0.4.8</t>
   </si>
   <si>
     <t xml:space="preserve">gorkathebot</t>
@@ -803,6 +803,150 @@
   </si>
   <si>
     <t xml:space="preserve">txt_hdi_links</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take a look at {lnk_hdi_google} and {lnk_hdi_wikipedia}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rem_hdi_section_end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MENUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAGICVARS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIMITIVES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StrReplace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strFrom strTo strSubject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strResult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SplitToArray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strSeparator strString</t>
+  </si>
+  <si>
+    <t xml:space="preserve">...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DiffPipeArrays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strPipedArrayFrom strPipedArrayMinus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strPipedArrayDiff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StrPosOf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strHaystack strNeedle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intPos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">returns -1 if not found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SubStr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strString, intStart, intLength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strSubstring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StrToLower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strString</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strLowercased</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StrToUpper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strUppercased</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UrlEncode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strUrlencoded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Howdoi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROGRAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/echo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">echo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET oldBotMode botMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET botMode 99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINT ENTRYTEXT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">END</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/noecho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noecho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET botMode oldBotMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLEAR oldBotMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/.+/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">everything</t>
   </si>
   <si>
     <r>
@@ -812,7 +956,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Take a look at </t>
+      <t xml:space="preserve">IF NEQ botMode 99 THEN GOTO </t>
     </r>
     <r>
       <rPr>
@@ -820,130 +964,23 @@
         <rFont val="Liberation Sans Narrow"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">{lnk_hdi_google}</t>
+      <t xml:space="preserve">everything2</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Liberation Sans Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Liberation Sans Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">{lnk_hdi_wikipedia}</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">rem_hdi_section_end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MENUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAGICVARS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIMITIVES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StrReplace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strFrom strTo strSubject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strResult</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SplitToArray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strSeparator strString</t>
-  </si>
-  <si>
-    <t xml:space="preserve">...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DiffPipeArrays</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strPipedArrayFrom strPipedArrayMinus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strPipedArrayDiff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StrPosOf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strHaystack strNeedle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intPos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">returns -1 if not found</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SubStr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strString, intStart, intLength</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strSubstring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StrToLower</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strString</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strLowercased</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StrToUpper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strUppercased</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UrlEncode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strUrlencoded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Howdoi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">strA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROGRAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//</t>
+  </si>
+  <si>
+    <t xml:space="preserve">everything2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET type ENTRYTYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET id ENTRYID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINT mediaInfo</t>
   </si>
   <si>
     <t xml:space="preserve">/start</t>
@@ -961,9 +998,6 @@
     <t xml:space="preserve">IF EQ botMode optHowdoiBot THEN GOTO howdoi</t>
   </si>
   <si>
-    <t xml:space="preserve">END</t>
-  </si>
-  <si>
     <t xml:space="preserve">/oldstart</t>
   </si>
   <si>
@@ -1096,18 +1130,6 @@
     <t xml:space="preserve">PRINT sendMedia</t>
   </si>
   <si>
-    <t xml:space="preserve">//</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET type ENTRYTYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SET id ENTRYID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRINT mediaInfo</t>
-  </si>
-  <si>
     <t xml:space="preserve">/letmeask1</t>
   </si>
   <si>
@@ -1705,23 +1727,7 @@
     <t xml:space="preserve">GOSUB hdi_filter iaskthis TO filter</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Liberation Sans Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">IF EQ filter </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Liberation Sans Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">txt_hdi_filter_start THEN GOTO start</t>
-    </r>
+    <t xml:space="preserve">IF EQ filter txt_hdi_filter_start THEN GOTO start</t>
   </si>
   <si>
     <t xml:space="preserve">SET answered 1</t>
@@ -1799,42 +1805,10 @@
     <t xml:space="preserve">ARGS q</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Liberation Sans Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">IF EQ q txt_hdi_filter_start THEN RETURN </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Liberation Sans Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">txt_hdi_filter_start</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Liberation Sans Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">IF NEQ q </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Liberation Sans Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">txt_hdi_filter_die THEN GOTO hdi_filter_end</t>
-    </r>
+    <t xml:space="preserve">IF EQ q txt_hdi_filter_start THEN RETURN txt_hdi_filter_start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF NEQ q txt_hdi_filter_die THEN GOTO hdi_filter_end</t>
   </si>
   <si>
     <t xml:space="preserve">PRINT txt_hdi_dont_die</t>
@@ -1876,23 +1850,7 @@
     <t xml:space="preserve">CALL UrlEncode q TO q</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Liberation Sans Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">PRINT </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Liberation Sans Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">txt_hdi_links</t>
-    </r>
+    <t xml:space="preserve">PRINT txt_hdi_links</t>
   </si>
 </sst>
 </file>
@@ -1998,7 +1956,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2028,10 +1986,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2112,10 +2066,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P541"/>
+  <dimension ref="A1:P555"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A136" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C149" activeCellId="0" sqref="C149"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3181,7 +3135,7 @@
       </c>
     </row>
     <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="8" t="s">
+      <c r="A143" s="1" t="s">
         <v>246</v>
       </c>
       <c r="C143" s="1" t="s">
@@ -3189,7 +3143,7 @@
       </c>
     </row>
     <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="8" t="s">
+      <c r="A144" s="1" t="s">
         <v>248</v>
       </c>
       <c r="C144" s="1" t="s">
@@ -3197,7 +3151,7 @@
       </c>
     </row>
     <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="8" t="s">
+      <c r="A145" s="1" t="s">
         <v>250</v>
       </c>
       <c r="C145" s="1" t="s">
@@ -3213,7 +3167,7 @@
       </c>
     </row>
     <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="8" t="s">
+      <c r="A147" s="1" t="s">
         <v>254</v>
       </c>
       <c r="C147" s="1" t="s">
@@ -3221,15 +3175,15 @@
       </c>
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="8" t="s">
+      <c r="A148" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C148" s="8" t="s">
+      <c r="C148" s="1" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="8" t="s">
+      <c r="A149" s="1" t="s">
         <v>258</v>
       </c>
       <c r="C149" s="1" t="s">
@@ -3237,7 +3191,7 @@
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="8" t="s">
+      <c r="A150" s="1" t="s">
         <v>260</v>
       </c>
       <c r="C150" s="1" t="s">
@@ -3514,6 +3468,8 @@
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0"/>
+      <c r="B188" s="0"/>
       <c r="C188" s="1" t="s">
         <v>300</v>
       </c>
@@ -3528,7 +3484,9 @@
         <v>302</v>
       </c>
     </row>
-    <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0"/>
+    </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
         <v>303</v>
@@ -3541,131 +3499,147 @@
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0"/>
+      <c r="B193" s="0"/>
       <c r="C193" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C194" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C195" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="C195" s="1" t="s">
+    <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="1" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C196" s="1" t="s">
+      <c r="B197" s="1" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C197" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
     <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B198" s="1" t="s">
+      <c r="C198" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C199" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="C198" s="1" t="s">
+      <c r="B201" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C199" s="1" t="s">
+      <c r="C201" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C200" s="1" t="s">
+    <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C202" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C201" s="1" t="s">
+    <row r="203" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C203" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C202" s="1" t="s">
+    <row r="204" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C204" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B204" s="1" t="s">
+    <row r="205" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="206" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="C204" s="1" t="s">
+      <c r="B206" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C205" s="1" t="s">
+      <c r="C206" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C206" s="1" t="s">
+    <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C207" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C207" s="1" t="s">
+    <row r="208" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C208" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C208" s="1" t="s">
+    <row r="209" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C209" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="210" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="211" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="1" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C209" s="1" t="s">
+      <c r="B211" s="1" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C210" s="1" t="s">
+      <c r="C211" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B212" s="1" t="s">
+    <row r="212" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C212" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="213" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="214" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C212" s="1" t="s">
+      <c r="C214" s="1" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C213" s="1" t="s">
+    <row r="215" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C215" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C214" s="1" t="s">
+    <row r="216" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="217" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="1" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C215" s="1" t="s">
+      <c r="B217" s="1" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C216" s="1" t="s">
+      <c r="C217" s="1" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C217" s="1" t="s">
-        <v>322</v>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C218" s="1" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B219" s="1" t="s">
-        <v>329</v>
-      </c>
       <c r="C219" s="1" t="s">
         <v>330</v>
       </c>
@@ -3675,111 +3649,110 @@
         <v>331</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B222" s="1" t="s">
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C221" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B223" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C222" s="1" t="s">
+      <c r="C223" s="1" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C223" s="1" t="s">
-        <v>331</v>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C224" s="1" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B225" s="1" t="s">
-        <v>334</v>
-      </c>
       <c r="C225" s="1" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C226" s="1" t="s">
-        <v>331</v>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C227" s="1" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="C228" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C229" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C230" s="1" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B231" s="1" t="s">
+        <v>340</v>
+      </c>
       <c r="C231" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C232" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C233" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C234" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C235" s="1" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="B236" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="C236" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B238" s="1" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C237" s="1" t="s">
-        <v>302</v>
+      <c r="C238" s="1" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="1" t="s">
-        <v>347</v>
-      </c>
       <c r="C239" s="1" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C240" s="1" t="s">
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B241" s="1" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C241" s="1" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C242" s="1" t="s">
-        <v>302</v>
+        <v>348</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="1" t="s">
+      <c r="B244" s="1" t="s">
         <v>351</v>
       </c>
       <c r="C244" s="1" t="s">
@@ -3787,25 +3760,24 @@
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="0"/>
       <c r="C245" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C246" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="1" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C247" s="1" t="s">
         <v>354</v>
       </c>
     </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C248" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="1" t="s">
-        <v>355</v>
-      </c>
       <c r="C249" s="1" t="s">
         <v>356</v>
       </c>
@@ -3822,40 +3794,42 @@
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C252" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="C254" s="1" t="s">
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C253" s="1" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>362</v>
+      </c>
       <c r="C255" s="1" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C256" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C257" s="1" t="s">
-        <v>363</v>
+        <v>302</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="1" t="s">
+        <v>364</v>
+      </c>
       <c r="C258" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0"/>
       <c r="C259" s="1" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3868,203 +3842,198 @@
         <v>367</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C262" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="0"/>
+      <c r="A263" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="1" t="s">
-        <v>368</v>
-      </c>
       <c r="C264" s="1" t="s">
-        <v>352</v>
+        <v>370</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C265" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C266" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C267" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="1" t="s">
+        <v>372</v>
+      </c>
       <c r="C268" s="1" t="s">
-        <v>353</v>
+        <v>373</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C269" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C270" s="1" t="s">
-        <v>354</v>
+        <v>375</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B271" s="0"/>
+      <c r="C271" s="1" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B272" s="1" t="s">
-        <v>373</v>
-      </c>
       <c r="C272" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C273" s="1" t="s">
-        <v>331</v>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C274" s="1" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B275" s="1" t="s">
-        <v>375</v>
-      </c>
       <c r="C275" s="1" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C276" s="1" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C277" s="1" t="s">
-        <v>331</v>
-      </c>
+      <c r="A277" s="0"/>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="0"/>
+      <c r="A278" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="1" t="s">
-        <v>378</v>
-      </c>
       <c r="C279" s="1" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C280" s="1" t="s">
-        <v>354</v>
+        <v>383</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B281" s="0"/>
+      <c r="C281" s="1" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B282" s="1" t="s">
-        <v>380</v>
-      </c>
       <c r="C282" s="1" t="s">
-        <v>381</v>
+        <v>366</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C283" s="1" t="s">
-        <v>353</v>
+        <v>385</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C284" s="1" t="s">
-        <v>382</v>
+        <v>367</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C285" s="1" t="s">
-        <v>354</v>
+      <c r="B285" s="0"/>
+    </row>
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B286" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="1" t="s">
-        <v>383</v>
-      </c>
       <c r="C287" s="1" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C288" s="1" t="s">
-        <v>385</v>
+        <v>348</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B289" s="1" t="s">
+        <v>388</v>
+      </c>
       <c r="C289" s="1" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C290" s="1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C291" s="1" t="s">
-        <v>388</v>
+        <v>348</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C292" s="1" t="s">
-        <v>389</v>
-      </c>
+      <c r="A292" s="0"/>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="1" t="s">
+        <v>391</v>
+      </c>
       <c r="C293" s="1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C294" s="1" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C295" s="1" t="s">
-        <v>392</v>
-      </c>
+      <c r="B295" s="0"/>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B296" s="1" t="s">
+        <v>393</v>
+      </c>
       <c r="C296" s="1" t="s">
-        <v>382</v>
+        <v>394</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B297" s="1" t="s">
-        <v>393</v>
-      </c>
       <c r="C297" s="1" t="s">
-        <v>354</v>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C298" s="1" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="1" t="s">
-        <v>394</v>
-      </c>
       <c r="C299" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C300" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A301" s="1" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C301" s="1" t="s">
         <v>397</v>
       </c>
@@ -4096,860 +4065,872 @@
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C307" s="1" t="s">
-        <v>382</v>
+        <v>403</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C308" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C312" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C309" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C310" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B311" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="1" t="s">
-        <v>404</v>
-      </c>
       <c r="C314" s="1" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C315" s="1" t="s">
-        <v>302</v>
+        <v>410</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C316" s="1" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A317" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="B317" s="1" t="s">
-        <v>407</v>
-      </c>
       <c r="C317" s="1" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B318" s="1" t="s">
-        <v>409</v>
-      </c>
       <c r="C318" s="1" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C319" s="1" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C320" s="1" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C321" s="1" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C322" s="1" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C323" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B325" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="C325" s="1" t="s">
-        <v>416</v>
+        <v>367</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C326" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="1" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C327" s="1" t="s">
+      <c r="C328" s="1" t="s">
         <v>418</v>
-      </c>
-    </row>
-    <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C328" s="1" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C329" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B331" s="1" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C330" s="1" t="s">
+      <c r="C331" s="1" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C331" s="1" t="s">
-        <v>331</v>
+    <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B332" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B333" s="1" t="s">
-        <v>422</v>
-      </c>
       <c r="C333" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C334" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C335" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C336" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C337" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C338" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B339" s="1" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C339" s="1" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C340" s="1" t="s">
-        <v>331</v>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C341" s="1" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B342" s="1" t="s">
-        <v>430</v>
-      </c>
       <c r="C342" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C343" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C344" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B346" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="C346" s="1" t="s">
         <v>434</v>
       </c>
     </row>
+    <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C345" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B347" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B348" s="1" t="s">
-        <v>435</v>
-      </c>
       <c r="C348" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C349" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C350" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C351" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C352" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C353" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C354" s="1" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C355" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B356" s="1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C356" s="1" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C357" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B359" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="C359" s="1" t="s">
+    </row>
+    <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C358" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B360" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C360" s="1" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C361" s="1" t="s">
+    <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B362" s="1" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C362" s="1" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C363" s="1" t="s">
-        <v>382</v>
+        <v>450</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C364" s="1" t="s">
-        <v>331</v>
+        <v>451</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C365" s="1" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B366" s="1" t="s">
-        <v>450</v>
-      </c>
       <c r="C366" s="1" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C367" s="1" t="s">
-        <v>331</v>
+        <v>454</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C368" s="1" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B369" s="1" t="s">
-        <v>452</v>
-      </c>
       <c r="C369" s="1" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C370" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B372" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="C372" s="1" t="s">
-        <v>455</v>
+        <v>457</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C371" s="1" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B373" s="1" t="s">
+        <v>458</v>
+      </c>
       <c r="C373" s="1" t="s">
-        <v>331</v>
+        <v>459</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C374" s="1" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B375" s="1" t="s">
-        <v>456</v>
-      </c>
       <c r="C375" s="1" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C376" s="1" t="s">
-        <v>331</v>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C377" s="1" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B378" s="1" t="s">
-        <v>458</v>
-      </c>
       <c r="C378" s="1" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C379" s="1" t="s">
-        <v>331</v>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B380" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B381" s="1" t="s">
-        <v>460</v>
-      </c>
       <c r="C381" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C382" s="1" t="s">
-        <v>462</v>
+        <v>348</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B383" s="1" t="s">
+        <v>465</v>
+      </c>
       <c r="C383" s="1" t="s">
-        <v>429</v>
+        <v>466</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C384" s="1" t="s">
-        <v>331</v>
+        <v>348</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B386" s="1" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="C386" s="1" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C387" s="1" t="s">
-        <v>331</v>
+        <v>348</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B389" s="1" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="C389" s="1" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C390" s="1" t="s">
-        <v>331</v>
+        <v>348</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B392" s="1" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="C392" s="1" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C393" s="1" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C394" s="1" t="s">
-        <v>470</v>
+        <v>348</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B395" s="1" t="s">
+        <v>473</v>
+      </c>
       <c r="C395" s="1" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C396" s="1" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C397" s="1" t="s">
-        <v>473</v>
+        <v>442</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C398" s="1" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C399" s="1" t="s">
-        <v>331</v>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B400" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C400" s="1" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B401" s="1" t="s">
-        <v>475</v>
-      </c>
       <c r="C401" s="1" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C402" s="1" t="s">
-        <v>331</v>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B403" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C403" s="1" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B404" s="1" t="s">
-        <v>477</v>
-      </c>
       <c r="C404" s="1" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C405" s="1" t="s">
-        <v>478</v>
+        <v>348</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B406" s="1" t="s">
+        <v>480</v>
+      </c>
       <c r="C406" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C407" s="1" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C408" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C409" s="1" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C410" s="1" t="s">
-        <v>421</v>
+        <v>485</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C411" s="1" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C412" s="1" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C413" s="1" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C414" s="1" t="s">
-        <v>331</v>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B415" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C415" s="1" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B416" s="1" t="s">
-        <v>486</v>
-      </c>
       <c r="C416" s="1" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C417" s="1" t="s">
-        <v>331</v>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B418" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C418" s="1" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B419" s="1" t="s">
-        <v>488</v>
-      </c>
       <c r="C419" s="1" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C420" s="1" t="s">
-        <v>331</v>
+        <v>492</v>
+      </c>
+    </row>
+    <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C421" s="1" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B422" s="1" t="s">
-        <v>490</v>
-      </c>
       <c r="C422" s="1" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C423" s="1" t="s">
-        <v>331</v>
+        <v>495</v>
+      </c>
+    </row>
+    <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C424" s="1" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B425" s="1" t="s">
-        <v>492</v>
-      </c>
       <c r="C425" s="1" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C426" s="1" t="s">
-        <v>331</v>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C427" s="1" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B428" s="1" t="s">
-        <v>494</v>
-      </c>
       <c r="C428" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C429" s="1" t="s">
-        <v>331</v>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B430" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="C430" s="1" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B431" s="1" t="s">
-        <v>496</v>
-      </c>
       <c r="C431" s="1" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C432" s="1" t="s">
-        <v>497</v>
+        <v>348</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B433" s="1" t="s">
+        <v>501</v>
+      </c>
       <c r="C433" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B435" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="C435" s="1" t="s">
-        <v>436</v>
+        <v>502</v>
+      </c>
+    </row>
+    <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C434" s="1" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B436" s="1" t="s">
+        <v>503</v>
+      </c>
       <c r="C436" s="1" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C437" s="1" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C438" s="1" t="s">
-        <v>331</v>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B439" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C439" s="1" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B440" s="1" t="s">
-        <v>500</v>
-      </c>
       <c r="C440" s="1" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C441" s="1" t="s">
-        <v>502</v>
+        <v>348</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B442" s="1" t="s">
+        <v>507</v>
+      </c>
       <c r="C442" s="1" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C443" s="1" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C444" s="1" t="s">
-        <v>505</v>
+        <v>348</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B445" s="1" t="s">
+        <v>509</v>
+      </c>
       <c r="C445" s="1" t="s">
-        <v>429</v>
+        <v>449</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C446" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B448" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="C448" s="1" t="s">
-        <v>436</v>
+        <v>510</v>
+      </c>
+    </row>
+    <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C447" s="1" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B449" s="1" t="s">
+        <v>511</v>
+      </c>
       <c r="C449" s="1" t="s">
-        <v>507</v>
+        <v>449</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C450" s="1" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C451" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C452" s="1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C453" s="1" t="s">
-        <v>511</v>
+        <v>348</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B454" s="1" t="s">
+        <v>513</v>
+      </c>
       <c r="C454" s="1" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C455" s="1" t="s">
-        <v>331</v>
+        <v>515</v>
+      </c>
+    </row>
+    <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C456" s="1" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B457" s="1" t="s">
-        <v>513</v>
-      </c>
       <c r="C457" s="1" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C458" s="1" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C459" s="1" t="s">
-        <v>516</v>
+        <v>442</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C460" s="1" t="s">
-        <v>331</v>
+        <v>348</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B462" s="1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="C462" s="1" t="s">
-        <v>518</v>
+        <v>449</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C463" s="1" t="s">
-        <v>331</v>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C464" s="1" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B465" s="1" t="s">
-        <v>519</v>
-      </c>
       <c r="C465" s="1" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C466" s="1" t="s">
-        <v>331</v>
+        <v>523</v>
+      </c>
+    </row>
+    <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C467" s="1" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B468" s="1" t="s">
-        <v>521</v>
-      </c>
       <c r="C468" s="1" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C469" s="1" t="s">
-        <v>331</v>
+        <v>348</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B471" s="1" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="C471" s="1" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C472" s="1" t="s">
-        <v>331</v>
+        <v>528</v>
+      </c>
+    </row>
+    <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C473" s="1" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B474" s="1" t="s">
-        <v>525</v>
-      </c>
       <c r="C474" s="1" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C475" s="1" t="s">
-        <v>331</v>
+        <v>348</v>
+      </c>
+    </row>
+    <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B476" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="C476" s="1" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B477" s="1" t="s">
-        <v>527</v>
-      </c>
       <c r="C477" s="1" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C478" s="1" t="s">
-        <v>528</v>
+        <v>348</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B479" s="1" t="s">
+        <v>532</v>
+      </c>
       <c r="C479" s="1" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C480" s="1" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C481" s="1" t="s">
-        <v>531</v>
+        <v>348</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B482" s="1" t="s">
+        <v>534</v>
+      </c>
       <c r="C482" s="1" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C483" s="1" t="s">
-        <v>533</v>
+        <v>348</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B485" s="1" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="C485" s="1" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C486" s="1" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C487" s="1" t="s">
-        <v>537</v>
+        <v>348</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B488" s="1" t="s">
+        <v>538</v>
+      </c>
       <c r="C488" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C489" s="1" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C490" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B491" s="1" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C491" s="1" t="s">
-        <v>541</v>
+        <v>449</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C492" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C493" s="1" t="s">
         <v>542</v>
       </c>
     </row>
+    <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C494" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C495" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
     <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A496" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="B496" s="1" t="s">
-        <v>544</v>
-      </c>
       <c r="C496" s="1" t="s">
         <v>545</v>
       </c>
@@ -4959,199 +4940,189 @@
         <v>546</v>
       </c>
     </row>
-    <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B498" s="1" t="s">
+    <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B499" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="C498" s="1" t="s">
+      <c r="C499" s="1" t="s">
         <v>548</v>
-      </c>
-    </row>
-    <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C499" s="1" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C500" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C501" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C502" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C503" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C504" s="1" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C505" s="1" t="s">
         <v>554</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A506" s="1" t="s">
+      <c r="C506" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="B506" s="1" t="s">
+    </row>
+    <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A510" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="C506" s="1" t="s">
+      <c r="B510" s="1" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B507" s="1" t="s">
+      <c r="C510" s="1" t="s">
         <v>558</v>
       </c>
-      <c r="C507" s="1" t="s">
+    </row>
+    <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C511" s="1" t="s">
         <v>559</v>
-      </c>
-    </row>
-    <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C508" s="1" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C509" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C510" s="1" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B512" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C512" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C513" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C514" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C515" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C516" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C517" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C518" s="1" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A520" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B520" s="1" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B519" s="1" t="s">
+      <c r="C520" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="C519" s="1" t="s">
+    </row>
+    <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B521" s="1" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B520" s="1" t="s">
+      <c r="C521" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="C520" s="1" t="s">
+    </row>
+    <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C522" s="1" t="s">
         <v>573</v>
-      </c>
-    </row>
-    <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B522" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="C522" s="1" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C523" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C524" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B526" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="C526" s="1" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C527" s="1" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C525" s="8" t="s">
+    <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C528" s="1" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C526" s="8" t="s">
+    <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C529" s="1" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C527" s="8" t="s">
+    <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C530" s="1" t="s">
         <v>580</v>
-      </c>
-    </row>
-    <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B528" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="C528" s="1" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B530" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C530" s="1" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C531" s="1" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C532" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B533" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="C533" s="1" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B534" s="1" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C533" s="1" t="s">
+      <c r="C534" s="1" t="s">
         <v>586</v>
-      </c>
-    </row>
-    <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C534" s="1" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5159,32 +5130,101 @@
         <v>587</v>
       </c>
       <c r="C536" s="1" t="s">
-        <v>575</v>
+        <v>588</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C537" s="1" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C538" s="1" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C539" s="1" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C540" s="1" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C541" s="1" t="s">
-        <v>331</v>
+        <v>593</v>
+      </c>
+    </row>
+    <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B542" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="C542" s="1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B544" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="C544" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C545" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C546" s="1" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C547" s="1" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C548" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B550" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="C550" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C551" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C552" s="1" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C553" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C554" s="1" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C555" s="1" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix logic for PHOTO modifier
</commit_message>
<xml_diff>
--- a/_bots/gorkathebot/gorkathebot.xlsx
+++ b/_bots/gorkathebot/gorkathebot.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="620">
   <si>
     <t xml:space="preserve">BOTBASIC</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">VERSION</t>
   </si>
   <si>
-    <t xml:space="preserve">0.4.8</t>
+    <t xml:space="preserve">0.4.9</t>
   </si>
   <si>
     <t xml:space="preserve">gorkathebot</t>
@@ -811,6 +811,30 @@
     <t xml:space="preserve">rem_hdi_section_end</t>
   </si>
   <si>
+    <t xml:space="preserve">rem_feat_section_start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">featThese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/feat_photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thumbVideo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feats/video.mp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thumbPhoto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feats/photo.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rem_section_section_end</t>
+  </si>
+  <si>
     <t xml:space="preserve">MENUS</t>
   </si>
   <si>
@@ -949,23 +973,7 @@
     <t xml:space="preserve">everything</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Liberation Sans Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">IF NEQ botMode 99 THEN GOTO </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Liberation Sans Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">everything2</t>
-    </r>
+    <t xml:space="preserve">IF NEQ botMode 99 THEN GOTO everything2</t>
   </si>
   <si>
     <t xml:space="preserve">//</t>
@@ -1851,6 +1859,27 @@
   </si>
   <si>
     <t xml:space="preserve">PRINT txt_hdi_links</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/feat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINT featThese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLOAD thumbVideo TO vidId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLOAD thumbPhoto TO vidThumbId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPLAY vidId PHOTO vidThumbId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOTO feat</t>
   </si>
 </sst>
 </file>
@@ -1860,7 +1889,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1901,11 +1930,6 @@
       <name val="Liberation Sans Narrow"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Liberation Sans Narrow"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2066,10 +2090,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P555"/>
+  <dimension ref="A1:P573"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A129" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A162" activeCellId="0" sqref="A162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3207,72 +3231,40 @@
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="3" t="s">
+    <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B156" s="4"/>
-      <c r="C156" s="4"/>
-      <c r="D156" s="5"/>
-      <c r="E156" s="4"/>
-      <c r="F156" s="4"/>
-      <c r="G156" s="4"/>
-      <c r="H156" s="5"/>
-      <c r="I156" s="4"/>
-      <c r="J156" s="4"/>
-      <c r="K156" s="4"/>
-      <c r="L156" s="5"/>
-      <c r="M156" s="4"/>
-      <c r="N156" s="4"/>
-      <c r="O156" s="4"/>
-      <c r="P156" s="5"/>
-    </row>
-    <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C157" s="1" t="s">
+    </row>
+    <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="E157" s="1" t="s">
+      <c r="C158" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="F157" s="1" t="s">
+    </row>
+    <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="G157" s="1" t="s">
+      <c r="C159" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="3" t="s">
+    <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B161" s="4"/>
-      <c r="C161" s="4"/>
-      <c r="D161" s="5"/>
-      <c r="E161" s="4"/>
-      <c r="F161" s="4"/>
-      <c r="G161" s="4"/>
-      <c r="H161" s="5"/>
-      <c r="I161" s="4"/>
-      <c r="J161" s="4"/>
-      <c r="K161" s="4"/>
-      <c r="L161" s="5"/>
-      <c r="M161" s="4"/>
-      <c r="N161" s="4"/>
-      <c r="O161" s="4"/>
-      <c r="P161" s="5"/>
-    </row>
+      <c r="C160" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3280,7 +3272,7 @@
     <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="3" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
@@ -3303,476 +3295,503 @@
         <v>9</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
     </row>
     <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F169" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="F170" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="1" t="s">
+    <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="E171" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="F171" s="1" t="s">
-        <v>278</v>
-      </c>
+      <c r="B171" s="4"/>
+      <c r="C171" s="4"/>
+      <c r="D171" s="5"/>
+      <c r="E171" s="4"/>
+      <c r="F171" s="4"/>
+      <c r="G171" s="4"/>
+      <c r="H171" s="5"/>
+      <c r="I171" s="4"/>
+      <c r="J171" s="4"/>
+      <c r="K171" s="4"/>
+      <c r="L171" s="5"/>
+      <c r="M171" s="4"/>
+      <c r="N171" s="4"/>
+      <c r="O171" s="4"/>
+      <c r="P171" s="5"/>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B176" s="4"/>
+      <c r="C176" s="4"/>
+      <c r="D176" s="5"/>
+      <c r="E176" s="4"/>
+      <c r="F176" s="4"/>
+      <c r="G176" s="4"/>
+      <c r="H176" s="5"/>
+      <c r="I176" s="4"/>
+      <c r="J176" s="4"/>
+      <c r="K176" s="4"/>
+      <c r="L176" s="5"/>
+      <c r="M176" s="4"/>
+      <c r="N176" s="4"/>
+      <c r="O176" s="4"/>
+      <c r="P176" s="5"/>
+    </row>
+    <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F177" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E179" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="E172" s="1" t="s">
+      <c r="F179" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="F172" s="1" t="s">
+    </row>
+    <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="G172" s="1" t="s">
+      <c r="E180" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="1" t="s">
+      <c r="F180" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E173" s="1" t="s">
+    </row>
+    <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="F173" s="1" t="s">
+      <c r="E181" s="1" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="1" t="s">
+      <c r="F181" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="E174" s="1" t="s">
+    </row>
+    <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="F174" s="1" t="s">
+      <c r="E182" s="1" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="1" t="s">
+      <c r="F182" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E175" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F175" s="1" t="s">
+      <c r="G182" s="1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="F176" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="F178" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="B182" s="4"/>
-      <c r="C182" s="4"/>
-      <c r="D182" s="5"/>
-      <c r="E182" s="4"/>
-      <c r="F182" s="4"/>
-      <c r="G182" s="4"/>
-      <c r="H182" s="5"/>
-      <c r="I182" s="4"/>
-      <c r="J182" s="4"/>
-      <c r="K182" s="4"/>
-      <c r="L182" s="5"/>
-      <c r="M182" s="4"/>
-      <c r="N182" s="4"/>
-      <c r="O182" s="4"/>
-      <c r="P182" s="5"/>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F183" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F184" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F185" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F186" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="B192" s="4"/>
+      <c r="C192" s="4"/>
+      <c r="D192" s="5"/>
+      <c r="E192" s="4"/>
+      <c r="F192" s="4"/>
+      <c r="G192" s="4"/>
+      <c r="H192" s="5"/>
+      <c r="I192" s="4"/>
+      <c r="J192" s="4"/>
+      <c r="K192" s="4"/>
+      <c r="L192" s="5"/>
+      <c r="M192" s="4"/>
+      <c r="N192" s="4"/>
+      <c r="O192" s="4"/>
+      <c r="P192" s="5"/>
+    </row>
+    <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B183" s="1" t="s">
+      <c r="B193" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C183" s="1" t="s">
+      <c r="C193" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="C187" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="0"/>
-      <c r="B188" s="0"/>
-      <c r="C188" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C189" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C190" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="0"/>
-    </row>
-    <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="C192" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="0"/>
-      <c r="B193" s="0"/>
-      <c r="C193" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C194" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C195" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
+    <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C197" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B197" s="1" t="s">
+    </row>
+    <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0"/>
+      <c r="B198" s="0"/>
+      <c r="C198" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="C197" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C198" s="1" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C199" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>309</v>
+      </c>
+    </row>
+    <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C200" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
     <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="B201" s="1" t="s">
+      <c r="A201" s="0"/>
+    </row>
+    <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="C201" s="1" t="s">
+      <c r="B202" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C202" s="1" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="203" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0"/>
+      <c r="B203" s="0"/>
       <c r="C203" s="1" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="204" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C204" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="205" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="206" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="205" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C205" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="206" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B206" s="1" t="s">
+      <c r="B207" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="C206" s="1" t="s">
+      <c r="C207" s="1" t="s">
         <v>317</v>
-      </c>
-    </row>
-    <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C207" s="1" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="208" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C208" s="1" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="209" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C209" s="1" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
     </row>
     <row r="210" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="211" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C211" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="C211" s="1" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="212" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C212" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="213" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>321</v>
+      </c>
+    </row>
+    <row r="213" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C213" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
     <row r="214" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="1" t="s">
+      <c r="C214" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="215" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="216" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C214" s="1" t="s">
+      <c r="B216" s="1" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="215" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C215" s="1" t="s">
+      <c r="C216" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="216" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="217" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="1" t="s">
+      <c r="C217" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B217" s="1" t="s">
+    </row>
+    <row r="218" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C218" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C217" s="1" t="s">
+    </row>
+    <row r="219" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C219" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="220" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="221" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C218" s="1" t="s">
+      <c r="B221" s="1" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C219" s="1" t="s">
+      <c r="C221" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C220" s="1" t="s">
+    <row r="222" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C222" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="223" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="224" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C221" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B223" s="1" t="s">
+      <c r="C224" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C223" s="1" t="s">
+    </row>
+    <row r="225" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C225" s="1" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C224" s="1" t="s">
+    <row r="226" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="227" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="1" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C225" s="1" t="s">
+      <c r="B227" s="1" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C226" s="1" t="s">
+      <c r="C227" s="1" t="s">
         <v>336</v>
-      </c>
-    </row>
-    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C227" s="1" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C228" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C229" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C230" s="1" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B231" s="1" t="s">
+      <c r="C231" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B233" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="C231" s="1" t="s">
+      <c r="C233" s="1" t="s">
         <v>341</v>
-      </c>
-    </row>
-    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C232" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C233" s="1" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C234" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C235" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C236" s="1" t="s">
-        <v>339</v>
+        <v>344</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C237" s="1" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B238" s="1" t="s">
+      <c r="C238" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="C238" s="1" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C239" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B241" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C241" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="C241" s="1" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C242" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C243" s="1" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B244" s="1" t="s">
-        <v>351</v>
-      </c>
       <c r="C244" s="1" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C245" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="C247" s="1" t="s">
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C246" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B248" s="1" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C248" s="1" t="s">
         <v>355</v>
       </c>
@@ -3782,87 +3801,84 @@
         <v>356</v>
       </c>
     </row>
-    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C250" s="1" t="s">
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B251" s="1" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C251" s="1" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C252" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B254" s="1" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C253" s="1" t="s">
+      <c r="C254" s="1" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="1" t="s">
+      <c r="C255" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="B255" s="1" t="s">
+      <c r="C257" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C255" s="1" t="s">
+    </row>
+    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C258" s="1" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C256" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="1" t="s">
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C259" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="C258" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="0"/>
-      <c r="C259" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C260" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C261" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C262" s="1" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="1" t="s">
+      <c r="C263" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="C263" s="1" t="s">
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="1" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C264" s="1" t="s">
+      <c r="B265" s="1" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C265" s="1" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C266" s="1" t="s">
-        <v>367</v>
+        <v>310</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3874,54 +3890,50 @@
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="0"/>
       <c r="C269" s="1" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C270" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C271" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="1" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C272" s="1" t="s">
+      <c r="C273" s="1" t="s">
         <v>377</v>
-      </c>
-    </row>
-    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C273" s="1" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C274" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C275" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C276" s="1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="0"/>
+        <v>375</v>
+      </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C278" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="C278" s="1" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3941,67 +3953,68 @@
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C282" s="1" t="s">
-        <v>366</v>
+        <v>385</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C283" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C284" s="1" t="s">
-        <v>367</v>
+        <v>387</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B285" s="0"/>
+      <c r="C285" s="1" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B286" s="1" t="s">
-        <v>386</v>
-      </c>
       <c r="C286" s="1" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C287" s="1" t="s">
-        <v>348</v>
+      <c r="A287" s="0"/>
+    </row>
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B289" s="1" t="s">
-        <v>388</v>
-      </c>
       <c r="C289" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C290" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C291" s="1" t="s">
-        <v>348</v>
+        <v>392</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="0"/>
+      <c r="C292" s="1" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="1" t="s">
-        <v>391</v>
-      </c>
       <c r="C293" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C294" s="1" t="s">
-        <v>367</v>
+        <v>375</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4009,314 +4022,320 @@
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B296" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C297" s="1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C298" s="1" t="s">
-        <v>395</v>
+        <v>356</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B299" s="1" t="s">
+        <v>396</v>
+      </c>
       <c r="C299" s="1" t="s">
-        <v>367</v>
+        <v>397</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C300" s="1" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="1" t="s">
-        <v>396</v>
-      </c>
       <c r="C301" s="1" t="s">
-        <v>397</v>
+        <v>356</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C302" s="1" t="s">
-        <v>398</v>
-      </c>
+      <c r="A302" s="0"/>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="1" t="s">
+        <v>399</v>
+      </c>
       <c r="C303" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C304" s="1" t="s">
-        <v>400</v>
+        <v>375</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C305" s="1" t="s">
+      <c r="B305" s="0"/>
+    </row>
+    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B306" s="1" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C306" s="1" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C307" s="1" t="s">
-        <v>403</v>
+        <v>374</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C308" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C309" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C311" s="1" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C310" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B311" s="1" t="s">
+    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C312" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="C311" s="1" t="s">
-        <v>367</v>
-      </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="1" t="s">
+      <c r="C313" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="C313" s="1" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C314" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C315" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C316" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C317" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C318" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C319" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C320" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B321" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="1" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C321" s="1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C322" s="1" t="s">
-        <v>367</v>
+      <c r="C323" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C324" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C325" s="1" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C326" s="1" t="s">
-        <v>416</v>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C327" s="1" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A328" s="1" t="s">
-        <v>417</v>
-      </c>
       <c r="C328" s="1" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C329" s="1" t="s">
-        <v>302</v>
+        <v>422</v>
+      </c>
+    </row>
+    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C330" s="1" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A331" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="B331" s="1" t="s">
-        <v>420</v>
-      </c>
       <c r="C331" s="1" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B332" s="1" t="s">
-        <v>422</v>
-      </c>
       <c r="C332" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C333" s="1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C334" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C335" s="1" t="s">
-        <v>426</v>
+        <v>375</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C336" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C339" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="1" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C337" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B339" s="1" t="s">
+      <c r="B341" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="C339" s="1" t="s">
+      <c r="C341" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C340" s="1" t="s">
+    <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B342" s="1" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C341" s="1" t="s">
+      <c r="C342" s="1" t="s">
         <v>431</v>
-      </c>
-    </row>
-    <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C342" s="1" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C343" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C344" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C345" s="1" t="s">
-        <v>348</v>
+        <v>434</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C346" s="1" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B347" s="1" t="s">
-        <v>435</v>
-      </c>
       <c r="C347" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B349" s="1" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C348" s="1" t="s">
+      <c r="C349" s="1" t="s">
         <v>437</v>
-      </c>
-    </row>
-    <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C349" s="1" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C350" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C351" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C352" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C353" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C354" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B356" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C355" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B357" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="C356" s="1" t="s">
+      <c r="C357" s="1" t="s">
         <v>444</v>
-      </c>
-    </row>
-    <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C357" s="1" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C358" s="1" t="s">
-        <v>348</v>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C359" s="1" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B360" s="1" t="s">
-        <v>446</v>
-      </c>
       <c r="C360" s="1" t="s">
         <v>447</v>
       </c>
     </row>
+    <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C361" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B362" s="1" t="s">
-        <v>448</v>
-      </c>
       <c r="C362" s="1" t="s">
         <v>449</v>
       </c>
@@ -4328,878 +4347,873 @@
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C364" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B366" s="1" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C365" s="1" t="s">
+      <c r="C366" s="1" t="s">
         <v>452</v>
-      </c>
-    </row>
-    <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C366" s="1" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C367" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C368" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B370" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C370" s="1" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C369" s="1" t="s">
+    <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B372" s="1" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C370" s="1" t="s">
+      <c r="C372" s="1" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C371" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B373" s="1" t="s">
+      <c r="C373" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="C373" s="1" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C374" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C375" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C376" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C377" s="1" t="s">
-        <v>395</v>
+        <v>462</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C378" s="1" t="s">
-        <v>348</v>
+        <v>463</v>
+      </c>
+    </row>
+    <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C379" s="1" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B380" s="1" t="s">
-        <v>463</v>
-      </c>
       <c r="C380" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C381" s="1" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B383" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C383" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C384" s="1" t="s">
-        <v>348</v>
+        <v>468</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C385" s="1" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B386" s="1" t="s">
-        <v>467</v>
-      </c>
       <c r="C386" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C387" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B389" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="C389" s="1" t="s">
-        <v>470</v>
+        <v>403</v>
+      </c>
+    </row>
+    <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C388" s="1" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B390" s="1" t="s">
+        <v>471</v>
+      </c>
       <c r="C390" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B392" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="C392" s="1" t="s">
         <v>472</v>
       </c>
     </row>
+    <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C391" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B393" s="1" t="s">
+        <v>473</v>
+      </c>
       <c r="C393" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B395" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="C395" s="1" t="s">
         <v>474</v>
       </c>
     </row>
+    <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C394" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B396" s="1" t="s">
+        <v>475</v>
+      </c>
       <c r="C396" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C397" s="1" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C398" s="1" t="s">
-        <v>348</v>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B399" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="C399" s="1" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B400" s="1" t="s">
-        <v>476</v>
-      </c>
       <c r="C400" s="1" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C401" s="1" t="s">
-        <v>348</v>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B402" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="C402" s="1" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B403" s="1" t="s">
-        <v>478</v>
-      </c>
       <c r="C403" s="1" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C404" s="1" t="s">
-        <v>348</v>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B405" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="C405" s="1" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B406" s="1" t="s">
-        <v>480</v>
-      </c>
       <c r="C406" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C407" s="1" t="s">
-        <v>482</v>
+        <v>450</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C408" s="1" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C409" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B410" s="1" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C410" s="1" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C411" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B413" s="1" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C412" s="1" t="s">
+      <c r="C413" s="1" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C413" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B415" s="1" t="s">
+    <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C414" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B416" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="C415" s="1" t="s">
+      <c r="C416" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C416" s="1" t="s">
-        <v>348</v>
+    <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C417" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B418" s="1" t="s">
-        <v>490</v>
-      </c>
       <c r="C418" s="1" t="s">
-        <v>449</v>
+        <v>491</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C419" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C420" s="1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C421" s="1" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C422" s="1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C423" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C424" s="1" t="s">
-        <v>434</v>
+        <v>356</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B425" s="1" t="s">
+        <v>496</v>
+      </c>
       <c r="C425" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C426" s="1" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C427" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B428" s="1" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C428" s="1" t="s">
-        <v>348</v>
+        <v>457</v>
+      </c>
+    </row>
+    <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C429" s="1" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B430" s="1" t="s">
-        <v>499</v>
-      </c>
       <c r="C430" s="1" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C431" s="1" t="s">
-        <v>348</v>
+        <v>501</v>
+      </c>
+    </row>
+    <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C432" s="1" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B433" s="1" t="s">
-        <v>501</v>
-      </c>
       <c r="C433" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C434" s="1" t="s">
-        <v>348</v>
+        <v>442</v>
+      </c>
+    </row>
+    <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C435" s="1" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B436" s="1" t="s">
-        <v>503</v>
-      </c>
       <c r="C436" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C437" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B439" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="C439" s="1" t="s">
         <v>506</v>
       </c>
     </row>
+    <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C438" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B440" s="1" t="s">
+        <v>507</v>
+      </c>
       <c r="C440" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B442" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="C442" s="1" t="s">
         <v>508</v>
       </c>
     </row>
+    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C441" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B443" s="1" t="s">
+        <v>509</v>
+      </c>
       <c r="C443" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B445" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="C445" s="1" t="s">
-        <v>449</v>
+        <v>510</v>
+      </c>
+    </row>
+    <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C444" s="1" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B446" s="1" t="s">
+        <v>511</v>
+      </c>
       <c r="C446" s="1" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C447" s="1" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B449" s="1" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="C449" s="1" t="s">
-        <v>449</v>
+        <v>514</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C450" s="1" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C451" s="1" t="s">
-        <v>510</v>
+        <v>356</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B452" s="1" t="s">
+        <v>515</v>
+      </c>
       <c r="C452" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B454" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="C454" s="1" t="s">
-        <v>514</v>
+        <v>516</v>
+      </c>
+    </row>
+    <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C453" s="1" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B455" s="1" t="s">
+        <v>517</v>
+      </c>
       <c r="C455" s="1" t="s">
-        <v>515</v>
+        <v>457</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C456" s="1" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C457" s="1" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C458" s="1" t="s">
-        <v>518</v>
+        <v>356</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B459" s="1" t="s">
+        <v>519</v>
+      </c>
       <c r="C459" s="1" t="s">
-        <v>442</v>
+        <v>457</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C460" s="1" t="s">
-        <v>348</v>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C461" s="1" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B462" s="1" t="s">
-        <v>519</v>
-      </c>
       <c r="C462" s="1" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C463" s="1" t="s">
-        <v>520</v>
+        <v>356</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B464" s="1" t="s">
+        <v>521</v>
+      </c>
       <c r="C464" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C465" s="1" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C466" s="1" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C467" s="1" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C468" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C469" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B471" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="C471" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C470" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B472" s="1" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C472" s="1" t="s">
-        <v>528</v>
+        <v>457</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C473" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C474" s="1" t="s">
-        <v>348</v>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C475" s="1" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B476" s="1" t="s">
-        <v>530</v>
-      </c>
       <c r="C476" s="1" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C477" s="1" t="s">
-        <v>348</v>
+        <v>532</v>
+      </c>
+    </row>
+    <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C478" s="1" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B479" s="1" t="s">
-        <v>532</v>
-      </c>
       <c r="C479" s="1" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C480" s="1" t="s">
-        <v>348</v>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B481" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C481" s="1" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B482" s="1" t="s">
-        <v>534</v>
-      </c>
       <c r="C482" s="1" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C483" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B485" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="C485" s="1" t="s">
         <v>537</v>
       </c>
     </row>
+    <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C484" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B486" s="1" t="s">
+        <v>538</v>
+      </c>
       <c r="C486" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B488" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="C488" s="1" t="s">
         <v>539</v>
       </c>
     </row>
+    <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C487" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
     <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B489" s="1" t="s">
+        <v>540</v>
+      </c>
       <c r="C489" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B491" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="C491" s="1" t="s">
-        <v>449</v>
+        <v>541</v>
+      </c>
+    </row>
+    <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C490" s="1" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B492" s="1" t="s">
+        <v>542</v>
+      </c>
       <c r="C492" s="1" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C493" s="1" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C494" s="1" t="s">
-        <v>543</v>
+        <v>356</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B495" s="1" t="s">
+        <v>544</v>
+      </c>
       <c r="C495" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C496" s="1" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C497" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B498" s="1" t="s">
         <v>546</v>
       </c>
+      <c r="C498" s="1" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B499" s="1" t="s">
-        <v>547</v>
-      </c>
       <c r="C499" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B501" s="1" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C500" s="1" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C501" s="1" t="s">
-        <v>550</v>
+        <v>457</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C502" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C503" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C504" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C505" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C506" s="1" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C507" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B509" s="1" t="s">
         <v>555</v>
       </c>
+      <c r="C509" s="1" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A510" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="B510" s="1" t="s">
+      <c r="C510" s="1" t="s">
         <v>557</v>
-      </c>
-      <c r="C510" s="1" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C511" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C512" s="1" t="s">
         <v>559</v>
-      </c>
-    </row>
-    <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B512" s="1" t="s">
-        <v>560</v>
-      </c>
-      <c r="C512" s="1" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C513" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C514" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C515" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C516" s="1" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C517" s="1" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C518" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="C520" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C521" s="1" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B522" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="B520" s="1" t="s">
+      <c r="C522" s="1" t="s">
         <v>569</v>
-      </c>
-      <c r="C520" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B521" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="C521" s="1" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C522" s="1" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C523" s="1" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C524" s="1" t="s">
-        <v>348</v>
+        <v>571</v>
+      </c>
+    </row>
+    <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C525" s="1" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B526" s="1" t="s">
-        <v>575</v>
-      </c>
       <c r="C526" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C527" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C528" s="1" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A530" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B530" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C530" s="1" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C529" s="1" t="s">
+    <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B531" s="1" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C530" s="1" t="s">
+      <c r="C531" s="1" t="s">
         <v>580</v>
-      </c>
-    </row>
-    <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C531" s="1" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C532" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C533" s="1" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B533" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="C533" s="1" t="s">
-        <v>584</v>
-      </c>
-    </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B534" s="1" t="s">
-        <v>585</v>
-      </c>
       <c r="C534" s="1" t="s">
-        <v>586</v>
+        <v>356</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B536" s="1" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="C536" s="1" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C537" s="1" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C538" s="1" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C539" s="1" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C540" s="1" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C541" s="1" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B542" s="1" t="s">
-        <v>594</v>
-      </c>
       <c r="C542" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
+      </c>
+    </row>
+    <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B543" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="C543" s="1" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B544" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="C544" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B546" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="C546" s="1" t="s">
         <v>596</v>
-      </c>
-      <c r="C544" s="1" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C545" s="1" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C546" s="1" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C547" s="1" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C548" s="1" t="s">
-        <v>593</v>
+        <v>598</v>
+      </c>
+    </row>
+    <row r="549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C549" s="1" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B550" s="1" t="s">
+      <c r="C550" s="1" t="s">
         <v>600</v>
-      </c>
-      <c r="C550" s="1" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5208,23 +5222,111 @@
       </c>
     </row>
     <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B552" s="1" t="s">
+        <v>602</v>
+      </c>
       <c r="C552" s="1" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C553" s="1" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B554" s="1" t="s">
+        <v>604</v>
+      </c>
       <c r="C554" s="1" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
     </row>
     <row r="555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C555" s="1" t="s">
-        <v>348</v>
+        <v>605</v>
+      </c>
+    </row>
+    <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C556" s="1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C557" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C558" s="1" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B560" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="C560" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C561" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C562" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C563" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C564" s="1" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C565" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A567" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="B567" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="C567" s="1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C568" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A570" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C570" s="1" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C571" s="1" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C572" s="1" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C573" s="1" t="s">
+        <v>619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix backlink in parser upload form result
</commit_message>
<xml_diff>
--- a/_bots/gorkathebot/gorkathebot.xlsx
+++ b/_bots/gorkathebot/gorkathebot.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">VERSION</t>
   </si>
   <si>
-    <t xml:space="preserve">0.4.9</t>
+    <t xml:space="preserve">0.4.10</t>
   </si>
   <si>
     <t xml:space="preserve">gorkathebot</t>
@@ -1135,7 +1135,7 @@
     <t xml:space="preserve">test</t>
   </si>
   <si>
-    <t xml:space="preserve">PRINT sendMedia</t>
+    <t xml:space="preserve">PRINT sendMedia featThese</t>
   </si>
   <si>
     <t xml:space="preserve">/letmeask1</t>
@@ -2092,8 +2092,8 @@
   </sheetPr>
   <dimension ref="A1:P573"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A129" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A162" activeCellId="0" sqref="A162"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
add PHOTO support in parser / add PHOTO usage in svitolinabot
</commit_message>
<xml_diff>
--- a/_bots/gorkathebot/gorkathebot.xlsx
+++ b/_bots/gorkathebot/gorkathebot.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="634">
   <si>
     <t xml:space="preserve">BOTBASIC</t>
   </si>
@@ -451,10 +451,19 @@
     <t xml:space="preserve">20180106_day6f_hl_elina_vs_aliaksandra-sasnovic_480p.m4v</t>
   </si>
   <si>
+    <t xml:space="preserve">vid_18all_seasonresume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eli_best_of_season_before_finals.mp4</t>
+  </si>
+  <si>
     <t xml:space="preserve">rem_svb_images</t>
   </si>
   <si>
-    <t xml:space="preserve">rem_svb_images_1</t>
+    <t xml:space="preserve">img_18all_wonthefinals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">won_the_finals.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">rem_svb_genericstrings</t>
@@ -466,6 +475,12 @@
     <t xml:space="preserve">svitolinabot/tennis/2018/brisbane/{fn_filename}</t>
   </si>
   <si>
+    <t xml:space="preserve">fn_ffn18all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">svitolinabot/tennis/2018/all/{fn_filename}</t>
+  </si>
+  <si>
     <t xml:space="preserve">prmMediatype</t>
   </si>
   <si>
@@ -658,6 +673,12 @@
     <t xml:space="preserve">Brisbane 2018</t>
   </si>
   <si>
+    <t xml:space="preserve">opt18whole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whole 2018</t>
+  </si>
+  <si>
     <t xml:space="preserve">txtWasAbye</t>
   </si>
   <si>
@@ -1318,6 +1339,9 @@
     <t xml:space="preserve">OPTION opt18brisbane GOSUB tt18brisbane</t>
   </si>
   <si>
+    <t xml:space="preserve">OPTION opt18whole GOSUB tt18whole</t>
+  </si>
+  <si>
     <t xml:space="preserve">MENU TITLE prmTournament TO tournament</t>
   </si>
   <si>
@@ -1666,6 +1690,74 @@
     <t xml:space="preserve">GOSUB tt18brisQD0 7</t>
   </si>
   <si>
+    <t xml:space="preserve">tt18whole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET fn_filename vid_18all_seasonresume</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">BLOAD </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">fn_ffn18all </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">AS video TO vid</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SET fn_filename img_18all_wonthefinals</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">BLOAD </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">fn_ffn18all </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">AS photo TO tid</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">DISPLAY vid PHOTO tid</t>
+  </si>
+  <si>
     <t xml:space="preserve">isThereContent</t>
   </si>
   <si>
@@ -1870,13 +1962,45 @@
     <t xml:space="preserve">PRINT featThese</t>
   </si>
   <si>
-    <t xml:space="preserve">BLOAD thumbVideo TO vidId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BLOAD thumbPhoto TO vidThumbId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DISPLAY vidId PHOTO vidThumbId</t>
+    <t xml:space="preserve">REM BLOAD thumbVideo TO vidId</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">REM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">BLOAD thumbPhoto TO vidThumbId</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">REM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Liberation Sans Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">DISPLAY vidId PHOTO vidThumbId</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">GOTO feat</t>
@@ -1889,7 +2013,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1930,6 +2054,11 @@
       <name val="Liberation Sans Narrow"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Liberation Sans Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1980,7 +2109,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2010,6 +2139,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2090,7 +2223,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P573"/>
+  <dimension ref="A1:P585"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -2736,1103 +2869,1117 @@
       <c r="A83" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="C83" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="84" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="86" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="87" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="88" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="89" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="90" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="91" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="93" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="94" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="95" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="96" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="97" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="98" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="99" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="100" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="101" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="102" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="103" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="104" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="105" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="106" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="107" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="119" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C123" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C125" s="7" t="s">
         <v>222</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C126" s="1" t="s">
         <v>224</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C127" s="7" t="s">
         <v>226</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C128" s="1" t="s">
         <v>228</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C129" s="7" t="s">
         <v>230</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C130" s="1" t="s">
         <v>232</v>
+      </c>
+      <c r="C130" s="7" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="131" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C131" s="7" t="s">
         <v>234</v>
       </c>
+      <c r="C131" s="1" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C132" s="7"/>
+      <c r="A132" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="133" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="135" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C134" s="7" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="135" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C135" s="7"/>
+    </row>
+    <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
+    <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>262</v>
+      </c>
+    </row>
+    <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>265</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
+    <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
+    <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
     <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>273</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
     <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="B166" s="4"/>
-      <c r="C166" s="4"/>
-      <c r="D166" s="5"/>
-      <c r="E166" s="4"/>
-      <c r="F166" s="4"/>
-      <c r="G166" s="4"/>
-      <c r="H166" s="5"/>
-      <c r="I166" s="4"/>
-      <c r="J166" s="4"/>
-      <c r="K166" s="4"/>
-      <c r="L166" s="5"/>
-      <c r="M166" s="4"/>
-      <c r="N166" s="4"/>
-      <c r="O166" s="4"/>
-      <c r="P166" s="5"/>
-    </row>
-    <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="1" t="s">
+    <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B169" s="4"/>
+      <c r="C169" s="4"/>
+      <c r="D169" s="5"/>
+      <c r="E169" s="4"/>
+      <c r="F169" s="4"/>
+      <c r="G169" s="4"/>
+      <c r="H169" s="5"/>
+      <c r="I169" s="4"/>
+      <c r="J169" s="4"/>
+      <c r="K169" s="4"/>
+      <c r="L169" s="5"/>
+      <c r="M169" s="4"/>
+      <c r="N169" s="4"/>
+      <c r="O169" s="4"/>
+      <c r="P169" s="5"/>
+    </row>
+    <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C167" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E167" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F167" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="G167" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="B171" s="4"/>
-      <c r="C171" s="4"/>
-      <c r="D171" s="5"/>
-      <c r="E171" s="4"/>
-      <c r="F171" s="4"/>
-      <c r="G171" s="4"/>
-      <c r="H171" s="5"/>
-      <c r="I171" s="4"/>
-      <c r="J171" s="4"/>
-      <c r="K171" s="4"/>
-      <c r="L171" s="5"/>
-      <c r="M171" s="4"/>
-      <c r="N171" s="4"/>
-      <c r="O171" s="4"/>
-      <c r="P171" s="5"/>
-    </row>
-    <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="1" t="s">
+      <c r="C170" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B174" s="4"/>
+      <c r="C174" s="4"/>
+      <c r="D174" s="5"/>
+      <c r="E174" s="4"/>
+      <c r="F174" s="4"/>
+      <c r="G174" s="4"/>
+      <c r="H174" s="5"/>
+      <c r="I174" s="4"/>
+      <c r="J174" s="4"/>
+      <c r="K174" s="4"/>
+      <c r="L174" s="5"/>
+      <c r="M174" s="4"/>
+      <c r="N174" s="4"/>
+      <c r="O174" s="4"/>
+      <c r="P174" s="5"/>
+    </row>
+    <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C172" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="B176" s="4"/>
-      <c r="C176" s="4"/>
-      <c r="D176" s="5"/>
-      <c r="E176" s="4"/>
-      <c r="F176" s="4"/>
-      <c r="G176" s="4"/>
-      <c r="H176" s="5"/>
-      <c r="I176" s="4"/>
-      <c r="J176" s="4"/>
-      <c r="K176" s="4"/>
-      <c r="L176" s="5"/>
-      <c r="M176" s="4"/>
-      <c r="N176" s="4"/>
-      <c r="O176" s="4"/>
-      <c r="P176" s="5"/>
-    </row>
-    <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E177" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F177" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="G177" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
+      <c r="C175" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F179" s="1" t="s">
-        <v>280</v>
-      </c>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B179" s="4"/>
+      <c r="C179" s="4"/>
+      <c r="D179" s="5"/>
+      <c r="E179" s="4"/>
+      <c r="F179" s="4"/>
+      <c r="G179" s="4"/>
+      <c r="H179" s="5"/>
+      <c r="I179" s="4"/>
+      <c r="J179" s="4"/>
+      <c r="K179" s="4"/>
+      <c r="L179" s="5"/>
+      <c r="M179" s="4"/>
+      <c r="N179" s="4"/>
+      <c r="O179" s="4"/>
+      <c r="P179" s="5"/>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F180" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="E180" s="1" t="s">
+      <c r="G180" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="F180" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="F181" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
+    </row>
+    <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F182" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="F182" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="G182" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>295</v>
       </c>
       <c r="F185" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
+      </c>
+      <c r="G185" s="1" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E186" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F187" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="E188" s="1" t="s">
         <v>302</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="B192" s="4"/>
-      <c r="C192" s="4"/>
-      <c r="D192" s="5"/>
-      <c r="E192" s="4"/>
-      <c r="F192" s="4"/>
-      <c r="G192" s="4"/>
-      <c r="H192" s="5"/>
-      <c r="I192" s="4"/>
-      <c r="J192" s="4"/>
-      <c r="K192" s="4"/>
-      <c r="L192" s="5"/>
-      <c r="M192" s="4"/>
-      <c r="N192" s="4"/>
-      <c r="O192" s="4"/>
-      <c r="P192" s="5"/>
-    </row>
-    <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="1" t="s">
+    <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B195" s="4"/>
+      <c r="C195" s="4"/>
+      <c r="D195" s="5"/>
+      <c r="E195" s="4"/>
+      <c r="F195" s="4"/>
+      <c r="G195" s="4"/>
+      <c r="H195" s="5"/>
+      <c r="I195" s="4"/>
+      <c r="J195" s="4"/>
+      <c r="K195" s="4"/>
+      <c r="L195" s="5"/>
+      <c r="M195" s="4"/>
+      <c r="N195" s="4"/>
+      <c r="O195" s="4"/>
+      <c r="P195" s="5"/>
+    </row>
+    <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B193" s="1" t="s">
+      <c r="B196" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C193" s="1" t="s">
+      <c r="C196" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="B197" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="C197" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="0"/>
-      <c r="B198" s="0"/>
-      <c r="C198" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C199" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
+    <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>313</v>
+      </c>
       <c r="C200" s="1" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0"/>
+      <c r="B201" s="0"/>
+      <c r="C201" s="1" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>312</v>
-      </c>
       <c r="C202" s="1" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="203" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="0"/>
-      <c r="B203" s="0"/>
       <c r="C203" s="1" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="204" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C204" s="1" t="s">
-        <v>309</v>
-      </c>
+      <c r="A204" s="0"/>
     </row>
     <row r="205" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>319</v>
+      </c>
       <c r="C205" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="206" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="206" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0"/>
+      <c r="B206" s="0"/>
+      <c r="C206" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
     <row r="207" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B207" s="1" t="s">
+      <c r="C207" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="C207" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="208" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C208" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="209" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C209" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="210" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="209" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="210" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
     <row r="211" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>319</v>
-      </c>
       <c r="C211" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="212" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C212" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="213" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C213" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="213" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="214" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="C214" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="215" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="215" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C215" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
     <row r="216" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>324</v>
-      </c>
       <c r="C216" s="1" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="217" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C217" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="218" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C218" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="218" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="219" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>331</v>
+      </c>
       <c r="C219" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="220" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>332</v>
+      </c>
+    </row>
+    <row r="220" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C220" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
     <row r="221" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>329</v>
-      </c>
       <c r="C221" s="1" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="222" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C222" s="1" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
     </row>
     <row r="223" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="224" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="s">
-        <v>331</v>
+        <v>335</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>336</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="225" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C225" s="1" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
     </row>
     <row r="226" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="227" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="B227" s="1" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="228" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C228" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C229" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="229" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="230" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>342</v>
+      </c>
       <c r="C230" s="1" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C231" s="1" t="s">
-        <v>310</v>
+        <v>344</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C232" s="1" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B233" s="1" t="s">
-        <v>340</v>
-      </c>
       <c r="C233" s="1" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C234" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C235" s="1" t="s">
-        <v>343</v>
+        <v>317</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B236" s="1" t="s">
+        <v>347</v>
+      </c>
       <c r="C236" s="1" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C237" s="1" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C238" s="1" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C239" s="1" t="s">
-        <v>347</v>
+        <v>351</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C240" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B241" s="1" t="s">
-        <v>348</v>
-      </c>
       <c r="C241" s="1" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C242" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C243" s="1" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B244" s="1" t="s">
+        <v>355</v>
+      </c>
       <c r="C244" s="1" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C245" s="1" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C246" s="1" t="s">
-        <v>347</v>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C247" s="1" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B248" s="1" t="s">
-        <v>354</v>
-      </c>
       <c r="C248" s="1" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C249" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B251" s="1" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C252" s="1" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B254" s="1" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C255" s="1" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="1" t="s">
-        <v>361</v>
+      <c r="B257" s="1" t="s">
+        <v>366</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3840,100 +3987,100 @@
         <v>363</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C259" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="1" t="s">
+        <v>368</v>
+      </c>
       <c r="C260" s="1" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C261" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C262" s="1" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C263" s="1" t="s">
-        <v>368</v>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C264" s="1" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="B265" s="1" t="s">
-        <v>370</v>
-      </c>
       <c r="C265" s="1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C266" s="1" t="s">
-        <v>310</v>
+        <v>375</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
-        <v>372</v>
+        <v>376</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>377</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="0"/>
       <c r="C269" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C270" s="1" t="s">
-        <v>374</v>
+        <v>317</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="1" t="s">
+        <v>379</v>
+      </c>
       <c r="C271" s="1" t="s">
-        <v>375</v>
+        <v>380</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="0"/>
+      <c r="C272" s="1" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="1" t="s">
-        <v>376</v>
-      </c>
       <c r="C273" s="1" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C274" s="1" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C275" s="1" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="1" t="s">
+        <v>383</v>
+      </c>
       <c r="C276" s="1" t="s">
-        <v>375</v>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C277" s="1" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="1" t="s">
-        <v>380</v>
-      </c>
       <c r="C278" s="1" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3941,1267 +4088,1262 @@
         <v>382</v>
       </c>
     </row>
-    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C280" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="C281" s="1" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C282" s="1" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C283" s="1" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C284" s="1" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C285" s="1" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C286" s="1" t="s">
-        <v>375</v>
+        <v>393</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="0"/>
+      <c r="C287" s="1" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="1" t="s">
-        <v>389</v>
-      </c>
       <c r="C288" s="1" t="s">
-        <v>373</v>
+        <v>395</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C289" s="1" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C290" s="1" t="s">
-        <v>391</v>
-      </c>
+      <c r="A290" s="0"/>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="1" t="s">
+        <v>396</v>
+      </c>
       <c r="C291" s="1" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C292" s="1" t="s">
-        <v>374</v>
+        <v>397</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C293" s="1" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C294" s="1" t="s">
-        <v>375</v>
+        <v>399</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B295" s="0"/>
+      <c r="C295" s="1" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B296" s="1" t="s">
-        <v>394</v>
-      </c>
       <c r="C296" s="1" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C297" s="1" t="s">
-        <v>356</v>
-      </c>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B298" s="0"/>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B299" s="1" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C300" s="1" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C301" s="1" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="0"/>
+      <c r="B302" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="1" t="s">
-        <v>399</v>
-      </c>
       <c r="C303" s="1" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C304" s="1" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B305" s="0"/>
+      <c r="A305" s="0"/>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B306" s="1" t="s">
-        <v>401</v>
+      <c r="A306" s="1" t="s">
+        <v>406</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C307" s="1" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C308" s="1" t="s">
-        <v>403</v>
-      </c>
+      <c r="B308" s="0"/>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B309" s="1" t="s">
+        <v>408</v>
+      </c>
       <c r="C309" s="1" t="s">
-        <v>375</v>
+        <v>409</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C310" s="1" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="1" t="s">
-        <v>404</v>
-      </c>
       <c r="C311" s="1" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C312" s="1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C313" s="1" t="s">
-        <v>407</v>
+        <v>382</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="1" t="s">
+        <v>411</v>
+      </c>
       <c r="C314" s="1" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C315" s="1" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C316" s="1" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C317" s="1" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C318" s="1" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C319" s="1" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C320" s="1" t="s">
-        <v>403</v>
+        <v>418</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B321" s="1" t="s">
-        <v>414</v>
-      </c>
       <c r="C321" s="1" t="s">
-        <v>375</v>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C322" s="1" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A323" s="1" t="s">
-        <v>415</v>
-      </c>
       <c r="C323" s="1" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B324" s="1" t="s">
+        <v>421</v>
+      </c>
       <c r="C324" s="1" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C325" s="1" t="s">
-        <v>418</v>
+        <v>382</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="1" t="s">
+        <v>422</v>
+      </c>
       <c r="C326" s="1" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C327" s="1" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C328" s="1" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C329" s="1" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C330" s="1" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C331" s="1" t="s">
-        <v>403</v>
+        <v>428</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C332" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C336" s="1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A338" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="C338" s="1" t="s">
-        <v>426</v>
+        <v>429</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C333" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C334" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C335" s="1" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C339" s="1" t="s">
-        <v>310</v>
+        <v>431</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="1" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B342" s="1" t="s">
-        <v>430</v>
-      </c>
       <c r="C342" s="1" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C343" s="1" t="s">
-        <v>432</v>
+        <v>317</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A344" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>435</v>
+      </c>
       <c r="C344" s="1" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B345" s="1" t="s">
+        <v>437</v>
+      </c>
       <c r="C345" s="1" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C346" s="1" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C347" s="1" t="s">
-        <v>368</v>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C348" s="1" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B349" s="1" t="s">
-        <v>436</v>
-      </c>
       <c r="C349" s="1" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C350" s="1" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C351" s="1" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C352" s="1" t="s">
-        <v>440</v>
+        <v>375</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B353" s="1" t="s">
+        <v>444</v>
+      </c>
       <c r="C353" s="1" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C354" s="1" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C355" s="1" t="s">
-        <v>356</v>
+        <v>447</v>
+      </c>
+    </row>
+    <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C356" s="1" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B357" s="1" t="s">
-        <v>443</v>
-      </c>
       <c r="C357" s="1" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C358" s="1" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C359" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C360" s="1" t="s">
-        <v>447</v>
+        <v>363</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B361" s="1" t="s">
+        <v>451</v>
+      </c>
       <c r="C361" s="1" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C362" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C363" s="1" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C364" s="1" t="s">
-        <v>356</v>
+        <v>455</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C365" s="1" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B366" s="1" t="s">
-        <v>451</v>
-      </c>
       <c r="C366" s="1" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C367" s="1" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C368" s="1" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B370" s="1" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="C370" s="1" t="s">
-        <v>455</v>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C371" s="1" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B372" s="1" t="s">
-        <v>456</v>
-      </c>
       <c r="C372" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C373" s="1" t="s">
-        <v>458</v>
+        <v>363</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B374" s="1" t="s">
+        <v>462</v>
+      </c>
       <c r="C374" s="1" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C375" s="1" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B376" s="1" t="s">
+        <v>464</v>
+      </c>
       <c r="C376" s="1" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C377" s="1" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C378" s="1" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C379" s="1" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C380" s="1" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C381" s="1" t="s">
-        <v>356</v>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C382" s="1" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B383" s="1" t="s">
-        <v>466</v>
-      </c>
       <c r="C383" s="1" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C384" s="1" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C385" s="1" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C386" s="1" t="s">
-        <v>470</v>
+        <v>363</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B387" s="1" t="s">
+        <v>474</v>
+      </c>
       <c r="C387" s="1" t="s">
-        <v>403</v>
+        <v>475</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C388" s="1" t="s">
-        <v>356</v>
+        <v>476</v>
+      </c>
+    </row>
+    <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C389" s="1" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B390" s="1" t="s">
-        <v>471</v>
-      </c>
       <c r="C390" s="1" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C391" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B393" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="C393" s="1" t="s">
-        <v>474</v>
+        <v>410</v>
+      </c>
+    </row>
+    <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C392" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B394" s="1" t="s">
+        <v>479</v>
+      </c>
       <c r="C394" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B396" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="C396" s="1" t="s">
-        <v>476</v>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C395" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B397" s="1" t="s">
+        <v>481</v>
+      </c>
       <c r="C397" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B399" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="C399" s="1" t="s">
-        <v>478</v>
+        <v>482</v>
+      </c>
+    </row>
+    <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C398" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B400" s="1" t="s">
+        <v>483</v>
+      </c>
       <c r="C400" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B402" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="C402" s="1" t="s">
-        <v>480</v>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C401" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B403" s="1" t="s">
+        <v>485</v>
+      </c>
       <c r="C403" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B405" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="C405" s="1" t="s">
-        <v>482</v>
+        <v>486</v>
+      </c>
+    </row>
+    <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C404" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B406" s="1" t="s">
+        <v>487</v>
+      </c>
       <c r="C406" s="1" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C407" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C408" s="1" t="s">
-        <v>356</v>
+        <v>363</v>
+      </c>
+    </row>
+    <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B409" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="C409" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B410" s="1" t="s">
-        <v>484</v>
-      </c>
       <c r="C410" s="1" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C411" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B413" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="C413" s="1" t="s">
-        <v>487</v>
+        <v>458</v>
+      </c>
+    </row>
+    <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C412" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B414" s="1" t="s">
+        <v>492</v>
+      </c>
       <c r="C414" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B416" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="C416" s="1" t="s">
-        <v>489</v>
+        <v>493</v>
+      </c>
+    </row>
+    <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C415" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B417" s="1" t="s">
+        <v>494</v>
+      </c>
       <c r="C417" s="1" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C418" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C419" s="1" t="s">
-        <v>492</v>
+        <v>363</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B420" s="1" t="s">
+        <v>496</v>
+      </c>
       <c r="C420" s="1" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C421" s="1" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C422" s="1" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C423" s="1" t="s">
-        <v>356</v>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C424" s="1" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B425" s="1" t="s">
-        <v>496</v>
-      </c>
       <c r="C425" s="1" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C426" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B428" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="C428" s="1" t="s">
-        <v>457</v>
+        <v>503</v>
+      </c>
+    </row>
+    <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C427" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B429" s="1" t="s">
+        <v>504</v>
+      </c>
       <c r="C429" s="1" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C430" s="1" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C431" s="1" t="s">
-        <v>501</v>
+        <v>363</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B432" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="C432" s="1" t="s">
-        <v>502</v>
+        <v>465</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C433" s="1" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C434" s="1" t="s">
-        <v>442</v>
+        <v>508</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C435" s="1" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C436" s="1" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C437" s="1" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C438" s="1" t="s">
-        <v>356</v>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C439" s="1" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B440" s="1" t="s">
-        <v>507</v>
-      </c>
       <c r="C440" s="1" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C441" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B443" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="C443" s="1" t="s">
-        <v>510</v>
+        <v>514</v>
+      </c>
+    </row>
+    <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C442" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B444" s="1" t="s">
+        <v>515</v>
+      </c>
       <c r="C444" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B446" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="C446" s="1" t="s">
-        <v>512</v>
+        <v>516</v>
+      </c>
+    </row>
+    <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C445" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B447" s="1" t="s">
+        <v>517</v>
+      </c>
       <c r="C447" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B449" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="C449" s="1" t="s">
-        <v>514</v>
+        <v>518</v>
+      </c>
+    </row>
+    <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C448" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B450" s="1" t="s">
+        <v>519</v>
+      </c>
       <c r="C450" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B452" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="C452" s="1" t="s">
-        <v>516</v>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C451" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B453" s="1" t="s">
+        <v>521</v>
+      </c>
       <c r="C453" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B455" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="C455" s="1" t="s">
-        <v>457</v>
+        <v>522</v>
+      </c>
+    </row>
+    <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C454" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B456" s="1" t="s">
+        <v>523</v>
+      </c>
       <c r="C456" s="1" t="s">
-        <v>518</v>
+        <v>524</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C457" s="1" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B459" s="1" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="C459" s="1" t="s">
-        <v>457</v>
+        <v>465</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C460" s="1" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C461" s="1" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C462" s="1" t="s">
-        <v>356</v>
+        <v>363</v>
+      </c>
+    </row>
+    <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B463" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="C463" s="1" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B464" s="1" t="s">
-        <v>521</v>
-      </c>
       <c r="C464" s="1" t="s">
-        <v>522</v>
+        <v>528</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C465" s="1" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C466" s="1" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C467" s="1" t="s">
-        <v>525</v>
+        <v>363</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B468" s="1" t="s">
+        <v>529</v>
+      </c>
       <c r="C468" s="1" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C469" s="1" t="s">
-        <v>450</v>
+        <v>531</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C470" s="1" t="s">
-        <v>356</v>
+        <v>532</v>
+      </c>
+    </row>
+    <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C471" s="1" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B472" s="1" t="s">
-        <v>527</v>
-      </c>
       <c r="C472" s="1" t="s">
-        <v>457</v>
+        <v>534</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C473" s="1" t="s">
-        <v>528</v>
+        <v>458</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C474" s="1" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C475" s="1" t="s">
-        <v>530</v>
+        <v>363</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B476" s="1" t="s">
+        <v>535</v>
+      </c>
       <c r="C476" s="1" t="s">
-        <v>531</v>
+        <v>465</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C477" s="1" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C478" s="1" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C479" s="1" t="s">
-        <v>356</v>
+        <v>538</v>
+      </c>
+    </row>
+    <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C480" s="1" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B481" s="1" t="s">
-        <v>534</v>
-      </c>
       <c r="C481" s="1" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C482" s="1" t="s">
-        <v>536</v>
+        <v>541</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C483" s="1" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C484" s="1" t="s">
-        <v>356</v>
+        <v>363</v>
+      </c>
+    </row>
+    <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B485" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C485" s="1" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B486" s="1" t="s">
-        <v>538</v>
-      </c>
       <c r="C486" s="1" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C487" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B489" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="C489" s="1" t="s">
-        <v>541</v>
+        <v>545</v>
+      </c>
+    </row>
+    <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C488" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B490" s="1" t="s">
+        <v>546</v>
+      </c>
       <c r="C490" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B492" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="C492" s="1" t="s">
-        <v>543</v>
+        <v>547</v>
+      </c>
+    </row>
+    <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C491" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B493" s="1" t="s">
+        <v>548</v>
+      </c>
       <c r="C493" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B495" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="C495" s="1" t="s">
-        <v>545</v>
+        <v>549</v>
+      </c>
+    </row>
+    <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C494" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B496" s="1" t="s">
+        <v>550</v>
+      </c>
       <c r="C496" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B498" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="C498" s="1" t="s">
-        <v>547</v>
+        <v>551</v>
+      </c>
+    </row>
+    <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C497" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B499" s="1" t="s">
+        <v>552</v>
+      </c>
       <c r="C499" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B501" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="C501" s="1" t="s">
-        <v>457</v>
+        <v>553</v>
+      </c>
+    </row>
+    <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C500" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B502" s="1" t="s">
+        <v>554</v>
+      </c>
       <c r="C502" s="1" t="s">
-        <v>549</v>
+        <v>555</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C503" s="1" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C504" s="1" t="s">
-        <v>551</v>
+        <v>363</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C505" s="1" t="s">
-        <v>552</v>
+      <c r="B505" s="8" t="s">
+        <v>556</v>
+      </c>
+      <c r="C505" s="8" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C506" s="1" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C507" s="1" t="s">
-        <v>554</v>
+      <c r="C507" s="8" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C508" s="1" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B509" s="1" t="s">
-        <v>555</v>
-      </c>
       <c r="C509" s="1" t="s">
-        <v>556</v>
+        <v>478</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C510" s="1" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C511" s="1" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C512" s="1" t="s">
-        <v>559</v>
+        <v>363</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B513" s="1" t="s">
+        <v>562</v>
+      </c>
       <c r="C513" s="1" t="s">
-        <v>560</v>
+        <v>465</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C514" s="1" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C515" s="1" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C516" s="1" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A520" s="1" t="s">
-        <v>564</v>
-      </c>
-      <c r="B520" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="C520" s="1" t="s">
+    </row>
+    <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C517" s="1" t="s">
         <v>566</v>
       </c>
     </row>
+    <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C518" s="1" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C519" s="1" t="s">
+        <v>568</v>
+      </c>
+    </row>
     <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B521" s="1" t="s">
+        <v>569</v>
+      </c>
       <c r="C521" s="1" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B522" s="1" t="s">
-        <v>568</v>
-      </c>
       <c r="C522" s="1" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
     </row>
     <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C523" s="1" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C524" s="1" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C525" s="1" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C526" s="1" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C527" s="1" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C528" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A530" s="1" t="s">
-        <v>576</v>
-      </c>
-      <c r="B530" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="C530" s="1" t="s">
+    </row>
+    <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A532" s="1" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B531" s="1" t="s">
+      <c r="B532" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="C531" s="1" t="s">
+      <c r="C532" s="1" t="s">
         <v>580</v>
-      </c>
-    </row>
-    <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C532" s="1" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C533" s="1" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B534" s="1" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C534" s="1" t="s">
-        <v>356</v>
+        <v>583</v>
+      </c>
+    </row>
+    <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C535" s="1" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B536" s="1" t="s">
-        <v>583</v>
-      </c>
       <c r="C536" s="1" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C537" s="1" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C538" s="1" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C539" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C540" s="1" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C541" s="1" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A542" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B542" s="1" t="s">
+        <v>591</v>
+      </c>
       <c r="C542" s="1" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B543" s="1" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="C543" s="1" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B544" s="1" t="s">
-        <v>593</v>
-      </c>
       <c r="C544" s="1" t="s">
-        <v>594</v>
+        <v>595</v>
+      </c>
+    </row>
+    <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C545" s="1" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B546" s="1" t="s">
-        <v>595</v>
-      </c>
       <c r="C546" s="1" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C547" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B548" s="1" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C548" s="1" t="s">
         <v>598</v>
       </c>
@@ -5222,120 +5364,184 @@
       </c>
     </row>
     <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B552" s="1" t="s">
+      <c r="C552" s="1" t="s">
         <v>602</v>
       </c>
-      <c r="C552" s="1" t="s">
+    </row>
+    <row r="553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C553" s="1" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B554" s="1" t="s">
+      <c r="C554" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="C554" s="1" t="s">
-        <v>596</v>
-      </c>
     </row>
     <row r="555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B555" s="1" t="s">
+        <v>605</v>
+      </c>
       <c r="C555" s="1" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B556" s="1" t="s">
+        <v>607</v>
+      </c>
       <c r="C556" s="1" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C557" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B558" s="1" t="s">
+        <v>609</v>
+      </c>
       <c r="C558" s="1" t="s">
-        <v>601</v>
+        <v>610</v>
+      </c>
+    </row>
+    <row r="559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C559" s="1" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B560" s="1" t="s">
-        <v>608</v>
-      </c>
       <c r="C560" s="1" t="s">
-        <v>596</v>
+        <v>612</v>
       </c>
     </row>
     <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C561" s="1" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
     </row>
     <row r="562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C562" s="1" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
     </row>
     <row r="563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C563" s="1" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
     </row>
     <row r="564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B564" s="1" t="s">
+        <v>616</v>
+      </c>
       <c r="C564" s="1" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C565" s="1" t="s">
-        <v>356</v>
+        <v>617</v>
+      </c>
+    </row>
+    <row r="566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B566" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="C566" s="1" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A567" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="B567" s="1" t="s">
-        <v>614</v>
-      </c>
       <c r="C567" s="1" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
     </row>
     <row r="568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C568" s="1" t="s">
-        <v>310</v>
+        <v>620</v>
+      </c>
+    </row>
+    <row r="569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C569" s="1" t="s">
+        <v>621</v>
       </c>
     </row>
     <row r="570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A570" s="1" t="s">
-        <v>265</v>
-      </c>
       <c r="C570" s="1" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C571" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B572" s="1" t="s">
+        <v>622</v>
+      </c>
       <c r="C572" s="1" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
     </row>
     <row r="573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C573" s="1" t="s">
-        <v>619</v>
+        <v>623</v>
+      </c>
+    </row>
+    <row r="574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C574" s="1" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C575" s="1" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C576" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="577" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C577" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A579" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="B579" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="C579" s="1" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="580" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C580" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A582" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C582" s="1" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="583" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C583" s="8" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="584" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C584" s="8" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C585" s="1" t="s">
+        <v>633</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C123" r:id="rId1" display="https://vk.com/@svitolina-elina-svitolina-s-kontoi-nam-predstoit-esche-odna-bitva"/>
-    <hyperlink ref="C125" r:id="rId2" display="http://svitolina.com/ru/news/456-news-04-01.html"/>
-    <hyperlink ref="C127" r:id="rId3" display="https://vk.com/@svitolina-elina-svitolina-taibreik-vo-vtorom-sete-ya-otygrala-na-vse-1"/>
-    <hyperlink ref="C129" r:id="rId4" display="https://vk.com/@svitolina-elina-svitolina-otkryvat-sezon-pobedoi-na-turnire-eto-vseg"/>
-    <hyperlink ref="C131" r:id="rId5" display="https://vk.com/@svitolina-elina-svitolina-nadeus-ya-horoshaya-aktrisa-i-vy-ne-zametili"/>
+    <hyperlink ref="C126" r:id="rId1" display="https://vk.com/@svitolina-elina-svitolina-s-kontoi-nam-predstoit-esche-odna-bitva"/>
+    <hyperlink ref="C128" r:id="rId2" display="http://svitolina.com/ru/news/456-news-04-01.html"/>
+    <hyperlink ref="C130" r:id="rId3" display="https://vk.com/@svitolina-elina-svitolina-taibreik-vo-vtorom-sete-ya-otygrala-na-vse-1"/>
+    <hyperlink ref="C132" r:id="rId4" display="https://vk.com/@svitolina-elina-svitolina-otkryvat-sezon-pobedoi-na-turnire-eto-vseg"/>
+    <hyperlink ref="C134" r:id="rId5" display="https://vk.com/@svitolina-elina-svitolina-nadeus-ya-horoshaya-aktrisa-i-vy-ne-zametili"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>